<commit_message>
Update to V3 for Gear Clamp and 30-Tooth Gear
</commit_message>
<xml_diff>
--- a/TurbofanDriver - V3 Bill of Materials.xlsx
+++ b/TurbofanDriver - V3 Bill of Materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/844add23945bcd8f/Documents/3D Printer Shit/1___3D_Printable_Jet_Engine_Upgrade/V3 Upgrades/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="865" documentId="13_ncr:1_{2F400004-E652-4E60-AF98-6B4D8D866B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20822795-022C-4B6E-B7C5-58E9AA2F87F0}"/>
+  <xr:revisionPtr revIDLastSave="868" documentId="13_ncr:1_{2F400004-E652-4E60-AF98-6B4D8D866B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24259998-EAF2-4569-9D4C-9A1311DAA952}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5160" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -166,12 +166,6 @@
   </si>
   <si>
     <t>HPT_-_V2</t>
-  </si>
-  <si>
-    <t>Gear_Clamp_-_V2</t>
-  </si>
-  <si>
-    <t>30_Tooth_Herringbone_Gear_-_V2</t>
   </si>
   <si>
     <t>Low_Pressure_Spool_Aft_-_V3</t>
@@ -531,6 +525,12 @@
   </si>
   <si>
     <t>B08H2HTTRT</t>
+  </si>
+  <si>
+    <t>30_Tooth_Herringbone_Gear_-_V3</t>
+  </si>
+  <si>
+    <t>Gear_Clamp_-_V3</t>
   </si>
 </sst>
 </file>
@@ -1786,10 +1786,10 @@
   <dimension ref="A1:L1077"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C33" sqref="C33"/>
+      <selection pane="bottomRight" activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1806,7 +1806,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="130" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C1" s="130"/>
       <c r="D1" s="130"/>
@@ -1845,7 +1845,7 @@
       </c>
       <c r="C4" s="108"/>
       <c r="G4" s="108" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H4" s="111" t="s">
         <v>5</v>
@@ -1860,7 +1860,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="3"/>
@@ -1880,7 +1880,7 @@
     <row r="6" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="142"/>
       <c r="C6" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D6" s="28"/>
       <c r="E6" s="3"/>
@@ -1913,7 +1913,7 @@
       <c r="A8" s="142"/>
       <c r="B8" s="1"/>
       <c r="C8" s="11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="34"/>
@@ -1950,7 +1950,7 @@
       <c r="A10" s="142"/>
       <c r="B10" s="1"/>
       <c r="C10" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="34"/>
@@ -1976,7 +1976,7 @@
     </row>
     <row r="12" spans="1:11" s="86" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="132" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B12" s="83"/>
       <c r="C12" s="112"/>
@@ -1999,10 +1999,10 @@
         <v>10</v>
       </c>
       <c r="J12" s="108" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K12" s="108" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -2023,13 +2023,13 @@
         <v>1</v>
       </c>
       <c r="C14" s="84" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D14" s="88" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="88" t="s">
         <v>51</v>
-      </c>
-      <c r="E14" s="88" t="s">
-        <v>53</v>
       </c>
       <c r="F14" s="18">
         <v>32.99</v>
@@ -2043,7 +2043,7 @@
         <v>36.948800000000006</v>
       </c>
       <c r="I14" s="87" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J14" s="89" t="s">
         <v>8</v>
@@ -2055,13 +2055,13 @@
         <v>1</v>
       </c>
       <c r="C15" s="84" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D15" s="88" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E15" s="88" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F15" s="18">
         <v>10.75</v>
@@ -2075,7 +2075,7 @@
         <v>12.040000000000001</v>
       </c>
       <c r="I15" s="90" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J15" s="89" t="s">
         <v>8</v>
@@ -2087,13 +2087,13 @@
         <v>1</v>
       </c>
       <c r="C16" s="84" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D16" s="88" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E16" s="88" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F16" s="18">
         <v>11.88</v>
@@ -2107,7 +2107,7 @@
         <v>13.305600000000002</v>
       </c>
       <c r="I16" s="87" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J16" s="89" t="s">
         <v>8</v>
@@ -2119,13 +2119,13 @@
         <v>1</v>
       </c>
       <c r="C17" s="84" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D17" s="88" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E17" s="88" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F17" s="18">
         <v>13.99</v>
@@ -2139,7 +2139,7 @@
         <v>15.668800000000001</v>
       </c>
       <c r="I17" s="87" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J17" s="89" t="s">
         <v>8</v>
@@ -2151,13 +2151,13 @@
         <v>1</v>
       </c>
       <c r="C18" s="84" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D18" s="88" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E18" s="88" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F18" s="18">
         <v>30.13</v>
@@ -2171,7 +2171,7 @@
         <v>33.745600000000003</v>
       </c>
       <c r="I18" s="87" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J18" s="89" t="s">
         <v>8</v>
@@ -2183,13 +2183,13 @@
         <v>1</v>
       </c>
       <c r="C19" s="84" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D19" s="88" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E19" s="88" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F19" s="18">
         <v>11.43</v>
@@ -2203,7 +2203,7 @@
         <v>12.801600000000001</v>
       </c>
       <c r="I19" s="87" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J19" s="89" t="s">
         <v>8</v>
@@ -2215,13 +2215,13 @@
         <v>1</v>
       </c>
       <c r="C20" s="84" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D20" s="88" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E20" s="88" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F20" s="18">
         <v>15.99</v>
@@ -2235,7 +2235,7 @@
         <v>17.908800000000003</v>
       </c>
       <c r="I20" s="87" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J20" s="89" t="s">
         <v>8</v>
@@ -2247,13 +2247,13 @@
         <v>1</v>
       </c>
       <c r="C21" s="84" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D21" s="88" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E21" s="88" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F21" s="18">
         <v>15.99</v>
@@ -2267,7 +2267,7 @@
         <v>17.908800000000003</v>
       </c>
       <c r="I21" s="87" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J21" s="89" t="s">
         <v>8</v>
@@ -2279,13 +2279,13 @@
         <v>1</v>
       </c>
       <c r="C22" s="84" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="88" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="88" t="s">
         <v>77</v>
-      </c>
-      <c r="D22" s="88" t="s">
-        <v>51</v>
-      </c>
-      <c r="E22" s="88" t="s">
-        <v>79</v>
       </c>
       <c r="F22" s="18">
         <v>19.989999999999998</v>
@@ -2299,7 +2299,7 @@
         <v>22.3888</v>
       </c>
       <c r="I22" s="87" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J22" s="89" t="s">
         <v>8</v>
@@ -2311,13 +2311,13 @@
         <v>1</v>
       </c>
       <c r="C23" s="84" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D23" s="88" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E23" s="88" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F23" s="18">
         <v>23.99</v>
@@ -2331,7 +2331,7 @@
         <v>26.8688</v>
       </c>
       <c r="I23" s="87" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J23" s="89" t="s">
         <v>8</v>
@@ -2355,13 +2355,13 @@
         <v>1</v>
       </c>
       <c r="C25" s="84" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D25" s="88" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E25" s="88" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F25" s="18">
         <f>9.99/0.75</f>
@@ -2376,13 +2376,13 @@
         <v>14.918400000000002</v>
       </c>
       <c r="I25" s="87" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J25" s="89" t="s">
         <v>8</v>
       </c>
       <c r="K25" s="90" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="L25" s="89" t="s">
         <v>8</v>
@@ -2406,13 +2406,13 @@
         <v>1</v>
       </c>
       <c r="C27" s="84" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="88" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" s="88" t="s">
         <v>63</v>
-      </c>
-      <c r="D27" s="88" t="s">
-        <v>64</v>
-      </c>
-      <c r="E27" s="88" t="s">
-        <v>65</v>
       </c>
       <c r="F27" s="18">
         <f>(6.65+8)/0.75</f>
@@ -2427,13 +2427,13 @@
         <v>21.877333333333336</v>
       </c>
       <c r="I27" s="87" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J27" s="87" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K27" s="90" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L27" s="89" t="s">
         <v>8</v>
@@ -2457,10 +2457,10 @@
         <v>1</v>
       </c>
       <c r="C29" s="84" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D29" s="88" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E29" s="101" t="s">
         <v>8</v>
@@ -2477,7 +2477,7 @@
         <v>11.200000000000001</v>
       </c>
       <c r="I29" s="102" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J29" s="89"/>
     </row>
@@ -2517,13 +2517,13 @@
         <v>1</v>
       </c>
       <c r="C32" s="84" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D32" s="88" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E32" s="88" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F32" s="18">
         <v>15.99</v>
@@ -2537,7 +2537,7 @@
         <v>17.908800000000003</v>
       </c>
       <c r="I32" s="87" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J32" s="89" t="s">
         <v>8</v>
@@ -2549,13 +2549,13 @@
         <v>1</v>
       </c>
       <c r="C33" s="84" t="s">
+        <v>142</v>
+      </c>
+      <c r="D33" s="88" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" s="88" t="s">
         <v>144</v>
-      </c>
-      <c r="D33" s="88" t="s">
-        <v>51</v>
-      </c>
-      <c r="E33" s="88" t="s">
-        <v>146</v>
       </c>
       <c r="F33" s="18">
         <v>12.99</v>
@@ -2569,7 +2569,7 @@
         <v>14.548800000000002</v>
       </c>
       <c r="I33" s="87" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J33" s="89" t="s">
         <v>8</v>
@@ -2581,13 +2581,13 @@
         <v>2</v>
       </c>
       <c r="C34" s="84" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D34" s="88" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E34" s="88" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F34" s="18">
         <v>9.9499999999999993</v>
@@ -2601,7 +2601,7 @@
         <v>22.288</v>
       </c>
       <c r="I34" s="87" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J34" s="89" t="s">
         <v>8</v>
@@ -2613,13 +2613,13 @@
         <v>2</v>
       </c>
       <c r="C35" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="D35" s="88" t="s">
+        <v>49</v>
+      </c>
+      <c r="E35" s="88" t="s">
         <v>87</v>
-      </c>
-      <c r="D35" s="88" t="s">
-        <v>51</v>
-      </c>
-      <c r="E35" s="88" t="s">
-        <v>89</v>
       </c>
       <c r="F35" s="18">
         <v>10.43</v>
@@ -2633,7 +2633,7 @@
         <v>23.363200000000003</v>
       </c>
       <c r="I35" s="87" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J35" s="89" t="s">
         <v>8</v>
@@ -2645,13 +2645,13 @@
         <v>1</v>
       </c>
       <c r="C36" s="84" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" s="88" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" s="88" t="s">
         <v>90</v>
-      </c>
-      <c r="D36" s="88" t="s">
-        <v>51</v>
-      </c>
-      <c r="E36" s="88" t="s">
-        <v>92</v>
       </c>
       <c r="F36" s="18">
         <v>9.99</v>
@@ -2665,7 +2665,7 @@
         <v>11.188800000000001</v>
       </c>
       <c r="I36" s="87" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J36" s="89" t="s">
         <v>8</v>
@@ -2691,13 +2691,13 @@
         <v>4</v>
       </c>
       <c r="C38" s="84" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D38" s="88" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E38" s="88" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F38" s="18">
         <v>1.6</v>
@@ -2711,7 +2711,7 @@
         <v>7.168000000000001</v>
       </c>
       <c r="I38" s="87" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J38" s="89" t="s">
         <v>8</v>
@@ -2737,7 +2737,7 @@
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="119" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D40" s="70"/>
       <c r="E40" s="70"/>
@@ -2781,7 +2781,7 @@
         <v>1</v>
       </c>
       <c r="C42" s="119" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D42" s="70"/>
       <c r="E42" s="70"/>
@@ -3336,10 +3336,10 @@
     <row r="66" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="139"/>
       <c r="B66" s="22" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C66" s="117" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D66" s="37"/>
       <c r="E66" s="35"/>
@@ -3351,10 +3351,10 @@
     <row r="67" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="139"/>
       <c r="B67" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C67" s="117" t="s">
         <v>134</v>
-      </c>
-      <c r="C67" s="117" t="s">
-        <v>136</v>
       </c>
       <c r="D67" s="37"/>
       <c r="E67" s="35"/>
@@ -3392,7 +3392,7 @@
         <v>1</v>
       </c>
       <c r="C69" s="117" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D69" s="37"/>
       <c r="E69" s="35"/>
@@ -3415,7 +3415,7 @@
         <v>1</v>
       </c>
       <c r="C70" s="117" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D70" s="37"/>
       <c r="E70" s="35"/>
@@ -3438,7 +3438,7 @@
         <v>1</v>
       </c>
       <c r="C71" s="32" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D71" s="37"/>
       <c r="E71" s="35"/>
@@ -3598,8 +3598,8 @@
       <c r="B78" s="22">
         <v>1</v>
       </c>
-      <c r="C78" s="32" t="s">
-        <v>45</v>
+      <c r="C78" s="117" t="s">
+        <v>146</v>
       </c>
       <c r="D78" s="37"/>
       <c r="E78" s="35"/>
@@ -3622,7 +3622,7 @@
         <v>1</v>
       </c>
       <c r="C79" s="117" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D79" s="37"/>
       <c r="E79" s="35"/>
@@ -3644,8 +3644,8 @@
       <c r="B80" s="22">
         <v>1</v>
       </c>
-      <c r="C80" s="32" t="s">
-        <v>46</v>
+      <c r="C80" s="117" t="s">
+        <v>145</v>
       </c>
       <c r="D80" s="37"/>
       <c r="E80" s="35"/>
@@ -3668,7 +3668,7 @@
         <v>1</v>
       </c>
       <c r="C81" s="117" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D81" s="37"/>
       <c r="E81" s="35"/>
@@ -3691,7 +3691,7 @@
         <v>1</v>
       </c>
       <c r="C82" s="117" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D82" s="37"/>
       <c r="E82" s="35"/>
@@ -3714,7 +3714,7 @@
         <v>1</v>
       </c>
       <c r="C83" s="32" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D83" s="37"/>
       <c r="E83" s="35"/>
@@ -3737,7 +3737,7 @@
         <v>1</v>
       </c>
       <c r="C84" s="32" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D84" s="37"/>
       <c r="E84" s="35"/>
@@ -3768,7 +3768,7 @@
     <row r="86" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="139"/>
       <c r="B86" s="144" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C86" s="145"/>
       <c r="D86" s="145"/>
@@ -3784,7 +3784,7 @@
         <v>1</v>
       </c>
       <c r="C87" s="118" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D87" s="54"/>
       <c r="E87" s="54"/>
@@ -3799,7 +3799,7 @@
         <v>1</v>
       </c>
       <c r="C88" s="118" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D88" s="54"/>
       <c r="E88" s="54"/>
@@ -3814,7 +3814,7 @@
         <v>1</v>
       </c>
       <c r="C89" s="117" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D89" s="37"/>
       <c r="E89" s="35"/>
@@ -3829,7 +3829,7 @@
         <v>1</v>
       </c>
       <c r="C90" s="117" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D90" s="37"/>
       <c r="E90" s="35"/>
@@ -3852,7 +3852,7 @@
         <v>1</v>
       </c>
       <c r="C91" s="117" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D91" s="37"/>
       <c r="E91" s="35"/>
@@ -3875,7 +3875,7 @@
         <v>1</v>
       </c>
       <c r="C92" s="117" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D92" s="37"/>
       <c r="E92" s="35"/>
@@ -3898,7 +3898,7 @@
         <v>1</v>
       </c>
       <c r="C93" s="117" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D93" s="37"/>
       <c r="E93" s="35"/>
@@ -3921,7 +3921,7 @@
         <v>1</v>
       </c>
       <c r="C94" s="117" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D94" s="37"/>
       <c r="E94" s="35"/>
@@ -3944,7 +3944,7 @@
         <v>1</v>
       </c>
       <c r="C95" s="117" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D95" s="37"/>
       <c r="E95" s="35"/>
@@ -3967,7 +3967,7 @@
         <v>1</v>
       </c>
       <c r="C96" s="117" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D96" s="37"/>
       <c r="E96" s="35"/>
@@ -3990,7 +3990,7 @@
         <v>1</v>
       </c>
       <c r="C97" s="117" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D97" s="37"/>
       <c r="E97" s="35"/>
@@ -4010,10 +4010,10 @@
     <row r="98" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="139"/>
       <c r="B98" s="22" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C98" s="117" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D98" s="37"/>
       <c r="E98" s="35"/>
@@ -4035,7 +4035,7 @@
         <v>1</v>
       </c>
       <c r="C99" s="117" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D99" s="37"/>
       <c r="E99" s="35"/>

</xml_diff>

<commit_message>
Update to power supply description and link
Clarified maximum dimensions and indicated greater than or equal to 4A supply required (can be 5 or 6 amp if available and correct size)
</commit_message>
<xml_diff>
--- a/TurbofanDriver - V3 Bill of Materials.xlsx
+++ b/TurbofanDriver - V3 Bill of Materials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/844add23945bcd8f/Documents/3D Printer Shit/1___3D_Printable_Jet_Engine_Upgrade/V3 Upgrades/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="882" documentId="13_ncr:1_{2F400004-E652-4E60-AF98-6B4D8D866B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F3865B7-24BB-4847-AE21-05A2C7861658}"/>
+  <xr:revisionPtr revIDLastSave="891" documentId="13_ncr:1_{2F400004-E652-4E60-AF98-6B4D8D866B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10524138-913A-4A90-BF33-61B00B2C2874}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="5160" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials - Rev 1" sheetId="3" r:id="rId1"/>
@@ -258,15 +258,6 @@
     <t>B09957G2VF</t>
   </si>
   <si>
-    <t>12V 4A Power Supply, AC Adapter 100-240V 50-60hz 12V 48W (&lt; 118mm long, 52mm wide, 32mm tall)</t>
-  </si>
-  <si>
-    <t>https://www.amazon.ca/Supply-Adapter-100-240V-Transformer-Camera-etc/dp/B086JNDVC5/</t>
-  </si>
-  <si>
-    <t>B086JNDVC5</t>
-  </si>
-  <si>
     <t>https://www.amazon.ca/BOJACK-Ceramic-Capacitor-Assortment-Capacitors/dp/B07P7HRGT9/</t>
   </si>
   <si>
@@ -310,9 +301,6 @@
   </si>
   <si>
     <t>Magnet Square - 0.25"</t>
-  </si>
-  <si>
-    <t>5A Rated Latching Push Button Switch 1NO1NC SPDT (or 1NO SPST) Black Metal Shell with Blue LED for 19mm 3/4"</t>
   </si>
   <si>
     <t>JLCPCB</t>
@@ -534,6 +522,18 @@
   </si>
   <si>
     <t>~137</t>
+  </si>
+  <si>
+    <t>4A Rated Latching Push Button Switch 1NO1NC SPDT (or 1NO SPST) Black Metal Shell with Blue LED for 19mm 3/4"</t>
+  </si>
+  <si>
+    <t>https://www.amazon.ca/gp/product/B09BQBWKKT/?th=1</t>
+  </si>
+  <si>
+    <t>12V ≥4A Power Supply, AC Adapter 100-240V 50-60hz (&lt; 125mm long, 55mm wide, 34mm tall)</t>
+  </si>
+  <si>
+    <t>B09BQBWKKT</t>
   </si>
 </sst>
 </file>
@@ -1584,10 +1584,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -1796,7 +1792,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N24" sqref="N24"/>
+      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1813,7 +1809,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="130" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C1" s="130"/>
       <c r="D1" s="130"/>
@@ -1852,7 +1848,7 @@
       </c>
       <c r="C4" s="108"/>
       <c r="G4" s="108" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H4" s="111" t="s">
         <v>5</v>
@@ -1867,7 +1863,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="3"/>
@@ -1877,7 +1873,7 @@
       </c>
       <c r="H5" s="128">
         <f xml:space="preserve"> H7+H9</f>
-        <v>368.59573333333338</v>
+        <v>370.83573333333339</v>
       </c>
       <c r="I5" s="109"/>
       <c r="J5" s="89" t="s">
@@ -1887,7 +1883,7 @@
     <row r="6" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="142"/>
       <c r="C6" s="11" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D6" s="28"/>
       <c r="E6" s="3"/>
@@ -1912,7 +1908,7 @@
       </c>
       <c r="H7" s="107">
         <f>SUM(H14:H29)</f>
-        <v>257.58133333333336</v>
+        <v>259.82133333333337</v>
       </c>
       <c r="I7" s="105"/>
     </row>
@@ -1920,7 +1916,7 @@
       <c r="A8" s="142"/>
       <c r="B8" s="1"/>
       <c r="C8" s="11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="34"/>
@@ -1957,7 +1953,7 @@
       <c r="A10" s="142"/>
       <c r="B10" s="1"/>
       <c r="C10" s="11" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="34"/>
@@ -1983,7 +1979,7 @@
     </row>
     <row r="12" spans="1:11" s="86" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="132" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B12" s="83"/>
       <c r="C12" s="112"/>
@@ -2006,10 +2002,10 @@
         <v>10</v>
       </c>
       <c r="J12" s="108" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="K12" s="108" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -2094,7 +2090,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="84" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D16" s="88" t="s">
         <v>49</v>
@@ -2126,13 +2122,13 @@
         <v>1</v>
       </c>
       <c r="C17" s="84" t="s">
-        <v>93</v>
+        <v>144</v>
       </c>
       <c r="D17" s="88" t="s">
         <v>49</v>
       </c>
       <c r="E17" s="88" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F17" s="18">
         <v>13.99</v>
@@ -2146,7 +2142,7 @@
         <v>15.668800000000001</v>
       </c>
       <c r="I17" s="87" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="J17" s="89" t="s">
         <v>8</v>
@@ -2286,27 +2282,27 @@
         <v>1</v>
       </c>
       <c r="C22" s="84" t="s">
-        <v>75</v>
+        <v>146</v>
       </c>
       <c r="D22" s="88" t="s">
         <v>49</v>
       </c>
       <c r="E22" s="88" t="s">
-        <v>77</v>
+        <v>147</v>
       </c>
       <c r="F22" s="18">
-        <v>19.989999999999998</v>
+        <v>21.99</v>
       </c>
       <c r="G22" s="4">
         <f t="shared" si="0"/>
-        <v>22.3888</v>
+        <v>24.628800000000002</v>
       </c>
       <c r="H22" s="16">
         <f t="shared" si="1"/>
-        <v>22.3888</v>
+        <v>24.628800000000002</v>
       </c>
       <c r="I22" s="87" t="s">
-        <v>76</v>
+        <v>145</v>
       </c>
       <c r="J22" s="89" t="s">
         <v>8</v>
@@ -2318,13 +2314,13 @@
         <v>1</v>
       </c>
       <c r="C23" s="84" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D23" s="88" t="s">
         <v>49</v>
       </c>
       <c r="E23" s="88" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F23" s="18">
         <v>23.99</v>
@@ -2338,7 +2334,7 @@
         <v>26.8688</v>
       </c>
       <c r="I23" s="87" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J23" s="89" t="s">
         <v>8</v>
@@ -2362,7 +2358,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="84" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D25" s="88" t="s">
         <v>60</v>
@@ -2389,7 +2385,7 @@
         <v>8</v>
       </c>
       <c r="K25" s="90" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="L25" s="89" t="s">
         <v>8</v>
@@ -2434,13 +2430,13 @@
         <v>21.877333333333336</v>
       </c>
       <c r="I27" s="87" t="s">
+        <v>129</v>
+      </c>
+      <c r="J27" s="87" t="s">
         <v>133</v>
       </c>
-      <c r="J27" s="87" t="s">
-        <v>137</v>
-      </c>
       <c r="K27" s="90" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="L27" s="89" t="s">
         <v>8</v>
@@ -2464,10 +2460,10 @@
         <v>1</v>
       </c>
       <c r="C29" s="84" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D29" s="88" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E29" s="101" t="s">
         <v>8</v>
@@ -2484,7 +2480,7 @@
         <v>11.200000000000001</v>
       </c>
       <c r="I29" s="102" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="J29" s="89"/>
     </row>
@@ -2524,13 +2520,13 @@
         <v>1</v>
       </c>
       <c r="C32" s="84" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D32" s="88" t="s">
         <v>49</v>
       </c>
       <c r="E32" s="88" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F32" s="18">
         <v>15.99</v>
@@ -2544,7 +2540,7 @@
         <v>17.908800000000003</v>
       </c>
       <c r="I32" s="87" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="J32" s="89" t="s">
         <v>8</v>
@@ -2553,16 +2549,16 @@
     <row r="33" spans="1:10" s="86" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="136"/>
       <c r="B33" s="88" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C33" s="84" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D33" s="88" t="s">
         <v>49</v>
       </c>
       <c r="E33" s="88" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F33" s="18">
         <v>12.99</v>
@@ -2576,7 +2572,7 @@
         <v>29.097600000000003</v>
       </c>
       <c r="I33" s="87" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="J33" s="89" t="s">
         <v>8</v>
@@ -2588,13 +2584,13 @@
         <v>2</v>
       </c>
       <c r="C34" s="84" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D34" s="88" t="s">
         <v>49</v>
       </c>
       <c r="E34" s="88" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F34" s="18">
         <v>9.9499999999999993</v>
@@ -2608,7 +2604,7 @@
         <v>22.288</v>
       </c>
       <c r="I34" s="87" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J34" s="89" t="s">
         <v>8</v>
@@ -2620,13 +2616,13 @@
         <v>2</v>
       </c>
       <c r="C35" s="84" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D35" s="88" t="s">
         <v>49</v>
       </c>
       <c r="E35" s="88" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F35" s="18">
         <v>10.43</v>
@@ -2640,7 +2636,7 @@
         <v>23.363200000000003</v>
       </c>
       <c r="I35" s="87" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J35" s="89" t="s">
         <v>8</v>
@@ -2652,13 +2648,13 @@
         <v>1</v>
       </c>
       <c r="C36" s="84" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D36" s="88" t="s">
         <v>49</v>
       </c>
       <c r="E36" s="88" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F36" s="18">
         <v>9.99</v>
@@ -2672,7 +2668,7 @@
         <v>11.188800000000001</v>
       </c>
       <c r="I36" s="87" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="J36" s="89" t="s">
         <v>8</v>
@@ -2698,13 +2694,13 @@
         <v>4</v>
       </c>
       <c r="C38" s="84" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D38" s="88" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E38" s="88" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F38" s="18">
         <v>1.6</v>
@@ -2718,7 +2714,7 @@
         <v>7.168000000000001</v>
       </c>
       <c r="I38" s="87" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="J38" s="89" t="s">
         <v>8</v>
@@ -2744,7 +2740,7 @@
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="119" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D40" s="70"/>
       <c r="E40" s="70"/>
@@ -2788,7 +2784,7 @@
         <v>1</v>
       </c>
       <c r="C42" s="119" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D42" s="70"/>
       <c r="E42" s="70"/>
@@ -3343,10 +3339,10 @@
     <row r="66" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="139"/>
       <c r="B66" s="22" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C66" s="117" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D66" s="37"/>
       <c r="E66" s="35"/>
@@ -3358,10 +3354,10 @@
     <row r="67" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="139"/>
       <c r="B67" s="22" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C67" s="117" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D67" s="37"/>
       <c r="E67" s="35"/>
@@ -3399,7 +3395,7 @@
         <v>1</v>
       </c>
       <c r="C69" s="117" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D69" s="37"/>
       <c r="E69" s="35"/>
@@ -3422,7 +3418,7 @@
         <v>1</v>
       </c>
       <c r="C70" s="117" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D70" s="37"/>
       <c r="E70" s="35"/>
@@ -3445,7 +3441,7 @@
         <v>1</v>
       </c>
       <c r="C71" s="32" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D71" s="37"/>
       <c r="E71" s="35"/>
@@ -3606,7 +3602,7 @@
         <v>1</v>
       </c>
       <c r="C78" s="117" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D78" s="37"/>
       <c r="E78" s="35"/>
@@ -3629,7 +3625,7 @@
         <v>1</v>
       </c>
       <c r="C79" s="117" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D79" s="37"/>
       <c r="E79" s="35"/>
@@ -3652,7 +3648,7 @@
         <v>1</v>
       </c>
       <c r="C80" s="117" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D80" s="37"/>
       <c r="E80" s="35"/>
@@ -3698,7 +3694,7 @@
         <v>1</v>
       </c>
       <c r="C82" s="117" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D82" s="37"/>
       <c r="E82" s="35"/>
@@ -3775,7 +3771,7 @@
     <row r="86" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="139"/>
       <c r="B86" s="144" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C86" s="145"/>
       <c r="D86" s="145"/>
@@ -3791,7 +3787,7 @@
         <v>1</v>
       </c>
       <c r="C87" s="118" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D87" s="54"/>
       <c r="E87" s="54"/>
@@ -3806,7 +3802,7 @@
         <v>1</v>
       </c>
       <c r="C88" s="118" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D88" s="54"/>
       <c r="E88" s="54"/>
@@ -3821,7 +3817,7 @@
         <v>1</v>
       </c>
       <c r="C89" s="117" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D89" s="37"/>
       <c r="E89" s="35"/>
@@ -3836,7 +3832,7 @@
         <v>1</v>
       </c>
       <c r="C90" s="117" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D90" s="37"/>
       <c r="E90" s="35"/>
@@ -3859,7 +3855,7 @@
         <v>1</v>
       </c>
       <c r="C91" s="117" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D91" s="37"/>
       <c r="E91" s="35"/>
@@ -3882,7 +3878,7 @@
         <v>1</v>
       </c>
       <c r="C92" s="117" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D92" s="37"/>
       <c r="E92" s="35"/>
@@ -3905,7 +3901,7 @@
         <v>1</v>
       </c>
       <c r="C93" s="117" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D93" s="37"/>
       <c r="E93" s="35"/>
@@ -3928,7 +3924,7 @@
         <v>1</v>
       </c>
       <c r="C94" s="117" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D94" s="37"/>
       <c r="E94" s="35"/>
@@ -3951,7 +3947,7 @@
         <v>1</v>
       </c>
       <c r="C95" s="117" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D95" s="37"/>
       <c r="E95" s="35"/>
@@ -3974,7 +3970,7 @@
         <v>1</v>
       </c>
       <c r="C96" s="117" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D96" s="37"/>
       <c r="E96" s="35"/>
@@ -3997,7 +3993,7 @@
         <v>1</v>
       </c>
       <c r="C97" s="117" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D97" s="37"/>
       <c r="E97" s="35"/>
@@ -4017,10 +4013,10 @@
     <row r="98" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="139"/>
       <c r="B98" s="22" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C98" s="117" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D98" s="37"/>
       <c r="E98" s="35"/>
@@ -4042,7 +4038,7 @@
         <v>1</v>
       </c>
       <c r="C99" s="117" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D99" s="37"/>
       <c r="E99" s="35"/>
@@ -14836,16 +14832,16 @@
     <hyperlink ref="I18" r:id="rId7" xr:uid="{49EDF83D-73DC-45CC-8EDD-D0A755D721E3}"/>
     <hyperlink ref="I20" r:id="rId8" xr:uid="{178D5D6A-78AD-4AB6-8C51-012C1D4D81AB}"/>
     <hyperlink ref="I21" r:id="rId9" xr:uid="{8DAE0086-1CB4-4A57-9E0C-FD0DC6DDE650}"/>
-    <hyperlink ref="I22" r:id="rId10" xr:uid="{2456F480-71EF-4AD3-A93F-EA30D00CD933}"/>
-    <hyperlink ref="I23" r:id="rId11" xr:uid="{0E7F6075-5095-4A84-859E-24E911CCA9A4}"/>
-    <hyperlink ref="I33" r:id="rId12" xr:uid="{1B9B6D2F-55F3-4431-803D-BCCE5374B90A}"/>
-    <hyperlink ref="I34" r:id="rId13" xr:uid="{7FC2CA57-66AA-443A-94C2-1F7E1E00ADB2}"/>
-    <hyperlink ref="I35" r:id="rId14" xr:uid="{A4957271-8C33-48E8-A6A4-18B6B9F48E67}"/>
-    <hyperlink ref="I36" r:id="rId15" xr:uid="{B760F12C-A43B-457F-A1FC-943FD6EC5069}"/>
-    <hyperlink ref="I38" r:id="rId16" xr:uid="{AD7CD1B5-E64B-46BD-9C45-7AFE1BA2261E}"/>
-    <hyperlink ref="K25" r:id="rId17" xr:uid="{4896C6AA-E74F-4FD2-94AF-03164218594A}"/>
-    <hyperlink ref="K27" r:id="rId18" xr:uid="{5304B522-7BFB-4401-9BB1-C7AF779A47B6}"/>
-    <hyperlink ref="J27" r:id="rId19" xr:uid="{DA1BC955-C30B-42D2-8DF9-55540D3C26E8}"/>
+    <hyperlink ref="I23" r:id="rId10" xr:uid="{0E7F6075-5095-4A84-859E-24E911CCA9A4}"/>
+    <hyperlink ref="I33" r:id="rId11" xr:uid="{1B9B6D2F-55F3-4431-803D-BCCE5374B90A}"/>
+    <hyperlink ref="I34" r:id="rId12" xr:uid="{7FC2CA57-66AA-443A-94C2-1F7E1E00ADB2}"/>
+    <hyperlink ref="I35" r:id="rId13" xr:uid="{A4957271-8C33-48E8-A6A4-18B6B9F48E67}"/>
+    <hyperlink ref="I36" r:id="rId14" xr:uid="{B760F12C-A43B-457F-A1FC-943FD6EC5069}"/>
+    <hyperlink ref="I38" r:id="rId15" xr:uid="{AD7CD1B5-E64B-46BD-9C45-7AFE1BA2261E}"/>
+    <hyperlink ref="K25" r:id="rId16" xr:uid="{4896C6AA-E74F-4FD2-94AF-03164218594A}"/>
+    <hyperlink ref="K27" r:id="rId17" xr:uid="{5304B522-7BFB-4401-9BB1-C7AF779A47B6}"/>
+    <hyperlink ref="J27" r:id="rId18" xr:uid="{DA1BC955-C30B-42D2-8DF9-55540D3C26E8}"/>
+    <hyperlink ref="I22" r:id="rId19" xr:uid="{2456F480-71EF-4AD3-A93F-EA30D00CD933}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Update list of V3 parts
Included V3 electronics bay cover to V3 list.
</commit_message>
<xml_diff>
--- a/TurbofanDriver - V3 Bill of Materials.xlsx
+++ b/TurbofanDriver - V3 Bill of Materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/844add23945bcd8f/Documents/3D Printer Shit/1___3D_Printable_Jet_Engine_Upgrade/V3 Upgrades/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="891" documentId="13_ncr:1_{2F400004-E652-4E60-AF98-6B4D8D866B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10524138-913A-4A90-BF33-61B00B2C2874}"/>
+  <xr:revisionPtr revIDLastSave="892" documentId="13_ncr:1_{2F400004-E652-4E60-AF98-6B4D8D866B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB678AD8-09DE-46D7-8513-BCDCFD419D9C}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5160" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>Turbofan Driver, Base/Electronics Assembly</t>
-  </si>
-  <si>
-    <t>Electronics_Bay_Cover_-_V2</t>
   </si>
   <si>
     <t>HPC_-_V2_-_10</t>
@@ -534,6 +531,9 @@
   </si>
   <si>
     <t>B09BQBWKKT</t>
+  </si>
+  <si>
+    <t>Electronics_Bay_Cover_-_V3</t>
   </si>
 </sst>
 </file>
@@ -1137,7 +1137,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1326,9 +1326,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1789,10 +1786,10 @@
   <dimension ref="A1:L1077"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
+      <selection pane="bottomRight" activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1808,36 +1805,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="130" t="s">
-        <v>100</v>
-      </c>
-      <c r="C1" s="130"/>
-      <c r="D1" s="130"/>
-      <c r="E1" s="130"/>
-      <c r="F1" s="130"/>
-      <c r="G1" s="130"/>
-      <c r="H1" s="130"/>
-      <c r="I1" s="130"/>
+      <c r="B1" s="129" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="129"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="129"/>
     </row>
     <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="130"/>
-      <c r="C2" s="130"/>
-      <c r="D2" s="130"/>
-      <c r="E2" s="130"/>
-      <c r="F2" s="130"/>
-      <c r="G2" s="130"/>
-      <c r="H2" s="130"/>
-      <c r="I2" s="130"/>
+      <c r="B2" s="129"/>
+      <c r="C2" s="129"/>
+      <c r="D2" s="129"/>
+      <c r="E2" s="129"/>
+      <c r="F2" s="129"/>
+      <c r="G2" s="129"/>
+      <c r="H2" s="129"/>
+      <c r="I2" s="129"/>
     </row>
     <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="131"/>
-      <c r="C3" s="131"/>
-      <c r="D3" s="131"/>
-      <c r="E3" s="131"/>
-      <c r="F3" s="131"/>
-      <c r="G3" s="131"/>
-      <c r="H3" s="131"/>
-      <c r="I3" s="131"/>
+      <c r="B3" s="130"/>
+      <c r="C3" s="130"/>
+      <c r="D3" s="130"/>
+      <c r="E3" s="130"/>
+      <c r="F3" s="130"/>
+      <c r="G3" s="130"/>
+      <c r="H3" s="130"/>
+      <c r="I3" s="130"/>
     </row>
     <row r="4" spans="1:11" s="31" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
@@ -1846,54 +1843,54 @@
       <c r="B4" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="108"/>
-      <c r="G4" s="108" t="s">
-        <v>98</v>
-      </c>
-      <c r="H4" s="111" t="s">
+      <c r="C4" s="107"/>
+      <c r="G4" s="107" t="s">
+        <v>97</v>
+      </c>
+      <c r="H4" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="110"/>
+      <c r="I4" s="109"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="141" t="s">
+      <c r="A5" s="140" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="3">
         <v>1</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="128">
+      <c r="G5" s="127">
         <v>250</v>
       </c>
-      <c r="H5" s="128">
+      <c r="H5" s="127">
         <f xml:space="preserve"> H7+H9</f>
         <v>370.83573333333339</v>
       </c>
-      <c r="I5" s="109"/>
-      <c r="J5" s="89" t="s">
+      <c r="I5" s="108"/>
+      <c r="J5" s="88" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="142"/>
+      <c r="A6" s="141"/>
       <c r="C6" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D6" s="28"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="129"/>
-      <c r="H6" s="129"/>
-      <c r="I6" s="106"/>
+      <c r="G6" s="128"/>
+      <c r="H6" s="128"/>
+      <c r="I6" s="105"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="142"/>
+      <c r="A7" s="141"/>
       <c r="B7" s="1">
         <v>1</v>
       </c>
@@ -1903,34 +1900,34 @@
       <c r="D7" s="13"/>
       <c r="E7" s="34"/>
       <c r="F7" s="34"/>
-      <c r="G7" s="103">
-        <v>0</v>
-      </c>
-      <c r="H7" s="107">
+      <c r="G7" s="102">
+        <v>0</v>
+      </c>
+      <c r="H7" s="106">
         <f>SUM(H14:H29)</f>
         <v>259.82133333333337</v>
       </c>
-      <c r="I7" s="105"/>
+      <c r="I7" s="104"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="142"/>
+      <c r="A8" s="141"/>
       <c r="B8" s="1"/>
       <c r="C8" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="34"/>
       <c r="F8" s="34"/>
-      <c r="G8" s="103">
+      <c r="G8" s="102">
         <v>160</v>
       </c>
-      <c r="H8" s="103">
-        <v>0</v>
-      </c>
-      <c r="I8" s="105"/>
+      <c r="H8" s="102">
+        <v>0</v>
+      </c>
+      <c r="I8" s="104"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="142"/>
+      <c r="A9" s="141"/>
       <c r="B9" s="1">
         <v>1</v>
       </c>
@@ -1940,99 +1937,99 @@
       <c r="D9" s="13"/>
       <c r="E9" s="34"/>
       <c r="F9" s="34"/>
-      <c r="G9" s="103">
-        <v>0</v>
-      </c>
-      <c r="H9" s="104">
+      <c r="G9" s="102">
+        <v>0</v>
+      </c>
+      <c r="H9" s="103">
         <f>SUM(H32:H38)</f>
         <v>111.01440000000002</v>
       </c>
-      <c r="I9" s="105"/>
+      <c r="I9" s="104"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="142"/>
+      <c r="A10" s="141"/>
       <c r="B10" s="1"/>
       <c r="C10" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="34"/>
       <c r="F10" s="34"/>
-      <c r="G10" s="103">
+      <c r="G10" s="102">
         <v>100</v>
       </c>
-      <c r="H10" s="103">
-        <v>0</v>
-      </c>
-      <c r="I10" s="105"/>
-    </row>
-    <row r="11" spans="1:11" s="75" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="143"/>
-      <c r="B11" s="71"/>
-      <c r="C11" s="76"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="72"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="74"/>
-    </row>
-    <row r="12" spans="1:11" s="86" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="132" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" s="83"/>
-      <c r="C12" s="112"/>
-      <c r="D12" s="108" t="s">
+      <c r="H10" s="102">
+        <v>0</v>
+      </c>
+      <c r="I10" s="104"/>
+    </row>
+    <row r="11" spans="1:11" s="74" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="142"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="75"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="72"/>
+      <c r="G11" s="71"/>
+      <c r="H11" s="72"/>
+      <c r="I11" s="73"/>
+    </row>
+    <row r="12" spans="1:11" s="85" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="131" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="82"/>
+      <c r="C12" s="111"/>
+      <c r="D12" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="108" t="s">
+      <c r="E12" s="107" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="113" t="s">
+      <c r="F12" s="112" t="s">
         <v>2</v>
       </c>
-      <c r="G12" s="113" t="s">
+      <c r="G12" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="H12" s="108" t="s">
+      <c r="H12" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="108" t="s">
+      <c r="I12" s="107" t="s">
         <v>10</v>
       </c>
-      <c r="J12" s="108" t="s">
-        <v>134</v>
-      </c>
-      <c r="K12" s="108" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="133"/>
-      <c r="B13" s="83"/>
-      <c r="C13" s="84"/>
-      <c r="D13" s="83"/>
-      <c r="E13" s="83"/>
+      <c r="J12" s="107" t="s">
+        <v>133</v>
+      </c>
+      <c r="K12" s="107" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="85" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="132"/>
+      <c r="B13" s="82"/>
+      <c r="C13" s="83"/>
+      <c r="D13" s="82"/>
+      <c r="E13" s="82"/>
       <c r="F13" s="16"/>
       <c r="G13" s="4"/>
       <c r="H13" s="16"/>
-      <c r="I13" s="85"/>
+      <c r="I13" s="84"/>
       <c r="J13"/>
     </row>
-    <row r="14" spans="1:11" s="86" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="133"/>
-      <c r="B14" s="83">
+    <row r="14" spans="1:11" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="132"/>
+      <c r="B14" s="82">
         <v>1</v>
       </c>
-      <c r="C14" s="84" t="s">
+      <c r="C14" s="83" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="87" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="88" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" s="88" t="s">
-        <v>51</v>
+      <c r="E14" s="87" t="s">
+        <v>50</v>
       </c>
       <c r="F14" s="18">
         <v>32.99</v>
@@ -2045,26 +2042,26 @@
         <f>B14*G14</f>
         <v>36.948800000000006</v>
       </c>
-      <c r="I14" s="87" t="s">
-        <v>50</v>
-      </c>
-      <c r="J14" s="89" t="s">
+      <c r="I14" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="J14" s="88" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="86" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="133"/>
-      <c r="B15" s="83">
+    <row r="15" spans="1:11" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="132"/>
+      <c r="B15" s="82">
         <v>1</v>
       </c>
-      <c r="C15" s="84" t="s">
+      <c r="C15" s="83" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="87" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="87" t="s">
         <v>56</v>
-      </c>
-      <c r="D15" s="88" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" s="88" t="s">
-        <v>57</v>
       </c>
       <c r="F15" s="18">
         <v>10.75</v>
@@ -2077,26 +2074,26 @@
         <f t="shared" ref="H15:H38" si="1">B15*G15</f>
         <v>12.040000000000001</v>
       </c>
-      <c r="I15" s="90" t="s">
-        <v>55</v>
-      </c>
-      <c r="J15" s="89" t="s">
+      <c r="I15" s="89" t="s">
+        <v>54</v>
+      </c>
+      <c r="J15" s="88" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="86" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="133"/>
-      <c r="B16" s="83">
+    <row r="16" spans="1:11" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="132"/>
+      <c r="B16" s="82">
         <v>1</v>
       </c>
-      <c r="C16" s="84" t="s">
-        <v>93</v>
-      </c>
-      <c r="D16" s="88" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" s="88" t="s">
-        <v>65</v>
+      <c r="C16" s="83" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="87" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="87" t="s">
+        <v>64</v>
       </c>
       <c r="F16" s="18">
         <v>11.88</v>
@@ -2109,26 +2106,26 @@
         <f t="shared" si="1"/>
         <v>13.305600000000002</v>
       </c>
-      <c r="I16" s="87" t="s">
-        <v>64</v>
-      </c>
-      <c r="J16" s="89" t="s">
+      <c r="I16" s="86" t="s">
+        <v>63</v>
+      </c>
+      <c r="J16" s="88" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="86" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="133"/>
-      <c r="B17" s="83">
+    <row r="17" spans="1:12" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="132"/>
+      <c r="B17" s="82">
         <v>1</v>
       </c>
-      <c r="C17" s="84" t="s">
-        <v>144</v>
-      </c>
-      <c r="D17" s="88" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" s="88" t="s">
-        <v>92</v>
+      <c r="C17" s="83" t="s">
+        <v>143</v>
+      </c>
+      <c r="D17" s="87" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="87" t="s">
+        <v>91</v>
       </c>
       <c r="F17" s="18">
         <v>13.99</v>
@@ -2141,26 +2138,26 @@
         <f t="shared" si="1"/>
         <v>15.668800000000001</v>
       </c>
-      <c r="I17" s="87" t="s">
-        <v>99</v>
-      </c>
-      <c r="J17" s="89" t="s">
+      <c r="I17" s="86" t="s">
+        <v>98</v>
+      </c>
+      <c r="J17" s="88" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="86" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="133"/>
-      <c r="B18" s="83">
+    <row r="18" spans="1:12" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="132"/>
+      <c r="B18" s="82">
         <v>1</v>
       </c>
-      <c r="C18" s="84" t="s">
-        <v>68</v>
-      </c>
-      <c r="D18" s="88" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" s="88" t="s">
+      <c r="C18" s="83" t="s">
         <v>67</v>
+      </c>
+      <c r="D18" s="87" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="87" t="s">
+        <v>66</v>
       </c>
       <c r="F18" s="18">
         <v>30.13</v>
@@ -2173,26 +2170,26 @@
         <f t="shared" si="1"/>
         <v>33.745600000000003</v>
       </c>
-      <c r="I18" s="87" t="s">
-        <v>66</v>
-      </c>
-      <c r="J18" s="89" t="s">
+      <c r="I18" s="86" t="s">
+        <v>65</v>
+      </c>
+      <c r="J18" s="88" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="86" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="133"/>
-      <c r="B19" s="83">
+    <row r="19" spans="1:12" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="132"/>
+      <c r="B19" s="82">
         <v>1</v>
       </c>
-      <c r="C19" s="84" t="s">
+      <c r="C19" s="83" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="87" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="87" t="s">
         <v>53</v>
-      </c>
-      <c r="D19" s="88" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" s="88" t="s">
-        <v>54</v>
       </c>
       <c r="F19" s="18">
         <v>11.43</v>
@@ -2205,26 +2202,26 @@
         <f t="shared" si="1"/>
         <v>12.801600000000001</v>
       </c>
-      <c r="I19" s="87" t="s">
-        <v>52</v>
-      </c>
-      <c r="J19" s="89" t="s">
+      <c r="I19" s="86" t="s">
+        <v>51</v>
+      </c>
+      <c r="J19" s="88" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="86" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="133"/>
-      <c r="B20" s="83">
+    <row r="20" spans="1:12" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="132"/>
+      <c r="B20" s="82">
         <v>1</v>
       </c>
-      <c r="C20" s="84" t="s">
+      <c r="C20" s="83" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="87" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="87" t="s">
         <v>70</v>
-      </c>
-      <c r="D20" s="88" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" s="88" t="s">
-        <v>71</v>
       </c>
       <c r="F20" s="18">
         <v>15.99</v>
@@ -2237,26 +2234,26 @@
         <f t="shared" si="1"/>
         <v>17.908800000000003</v>
       </c>
-      <c r="I20" s="87" t="s">
-        <v>69</v>
-      </c>
-      <c r="J20" s="89" t="s">
+      <c r="I20" s="86" t="s">
+        <v>68</v>
+      </c>
+      <c r="J20" s="88" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="86" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="133"/>
-      <c r="B21" s="83">
+    <row r="21" spans="1:12" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="132"/>
+      <c r="B21" s="82">
         <v>1</v>
       </c>
-      <c r="C21" s="84" t="s">
+      <c r="C21" s="83" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="87" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="87" t="s">
         <v>73</v>
-      </c>
-      <c r="D21" s="88" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" s="88" t="s">
-        <v>74</v>
       </c>
       <c r="F21" s="18">
         <v>15.99</v>
@@ -2269,26 +2266,26 @@
         <f t="shared" si="1"/>
         <v>17.908800000000003</v>
       </c>
-      <c r="I21" s="87" t="s">
-        <v>72</v>
-      </c>
-      <c r="J21" s="89" t="s">
+      <c r="I21" s="86" t="s">
+        <v>71</v>
+      </c>
+      <c r="J21" s="88" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="86" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="133"/>
-      <c r="B22" s="83">
+    <row r="22" spans="1:12" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="132"/>
+      <c r="B22" s="82">
         <v>1</v>
       </c>
-      <c r="C22" s="84" t="s">
+      <c r="C22" s="83" t="s">
+        <v>145</v>
+      </c>
+      <c r="D22" s="87" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="87" t="s">
         <v>146</v>
-      </c>
-      <c r="D22" s="88" t="s">
-        <v>49</v>
-      </c>
-      <c r="E22" s="88" t="s">
-        <v>147</v>
       </c>
       <c r="F22" s="18">
         <v>21.99</v>
@@ -2301,26 +2298,26 @@
         <f t="shared" si="1"/>
         <v>24.628800000000002</v>
       </c>
-      <c r="I22" s="87" t="s">
-        <v>145</v>
-      </c>
-      <c r="J22" s="89" t="s">
+      <c r="I22" s="86" t="s">
+        <v>144</v>
+      </c>
+      <c r="J22" s="88" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="86" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="133"/>
-      <c r="B23" s="83">
+    <row r="23" spans="1:12" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="132"/>
+      <c r="B23" s="82">
         <v>1</v>
       </c>
-      <c r="C23" s="84" t="s">
-        <v>77</v>
-      </c>
-      <c r="D23" s="88" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" s="88" t="s">
+      <c r="C23" s="83" t="s">
         <v>76</v>
+      </c>
+      <c r="D23" s="87" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="87" t="s">
+        <v>75</v>
       </c>
       <c r="F23" s="18">
         <v>23.99</v>
@@ -2333,38 +2330,38 @@
         <f t="shared" si="1"/>
         <v>26.8688</v>
       </c>
-      <c r="I23" s="87" t="s">
-        <v>75</v>
-      </c>
-      <c r="J23" s="89" t="s">
+      <c r="I23" s="86" t="s">
+        <v>74</v>
+      </c>
+      <c r="J23" s="88" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="86" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="133"/>
-      <c r="B24" s="83"/>
-      <c r="C24" s="84"/>
-      <c r="D24" s="88"/>
-      <c r="E24" s="88"/>
+    <row r="24" spans="1:12" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="132"/>
+      <c r="B24" s="82"/>
+      <c r="C24" s="83"/>
+      <c r="D24" s="87"/>
+      <c r="E24" s="87"/>
       <c r="F24" s="18"/>
       <c r="G24" s="4"/>
       <c r="H24" s="16"/>
-      <c r="I24" s="87"/>
-      <c r="J24" s="91"/>
-    </row>
-    <row r="25" spans="1:12" s="86" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="133"/>
-      <c r="B25" s="83">
+      <c r="I24" s="86"/>
+      <c r="J24" s="90"/>
+    </row>
+    <row r="25" spans="1:12" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="132"/>
+      <c r="B25" s="82">
         <v>1</v>
       </c>
-      <c r="C25" s="84" t="s">
-        <v>123</v>
-      </c>
-      <c r="D25" s="88" t="s">
-        <v>60</v>
-      </c>
-      <c r="E25" s="88" t="s">
+      <c r="C25" s="83" t="s">
+        <v>122</v>
+      </c>
+      <c r="D25" s="87" t="s">
         <v>59</v>
+      </c>
+      <c r="E25" s="87" t="s">
+        <v>58</v>
       </c>
       <c r="F25" s="18">
         <f>9.99/0.75</f>
@@ -2378,44 +2375,44 @@
         <f>B25*G25</f>
         <v>14.918400000000002</v>
       </c>
-      <c r="I25" s="87" t="s">
-        <v>58</v>
-      </c>
-      <c r="J25" s="89" t="s">
+      <c r="I25" s="86" t="s">
+        <v>57</v>
+      </c>
+      <c r="J25" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="K25" s="90" t="s">
-        <v>124</v>
-      </c>
-      <c r="L25" s="89" t="s">
+      <c r="K25" s="89" t="s">
+        <v>123</v>
+      </c>
+      <c r="L25" s="88" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="86" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="133"/>
-      <c r="B26" s="83"/>
-      <c r="C26" s="84"/>
-      <c r="D26" s="88"/>
-      <c r="E26" s="88"/>
+    <row r="26" spans="1:12" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="132"/>
+      <c r="B26" s="82"/>
+      <c r="C26" s="83"/>
+      <c r="D26" s="87"/>
+      <c r="E26" s="87"/>
       <c r="F26" s="18"/>
       <c r="G26" s="4"/>
       <c r="H26" s="16"/>
-      <c r="I26" s="87"/>
-      <c r="J26" s="91"/>
-    </row>
-    <row r="27" spans="1:12" s="86" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="133"/>
-      <c r="B27" s="83">
+      <c r="I26" s="86"/>
+      <c r="J26" s="90"/>
+    </row>
+    <row r="27" spans="1:12" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="132"/>
+      <c r="B27" s="82">
         <v>1</v>
       </c>
-      <c r="C27" s="84" t="s">
+      <c r="C27" s="83" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="87" t="s">
         <v>61</v>
       </c>
-      <c r="D27" s="88" t="s">
+      <c r="E27" s="87" t="s">
         <v>62</v>
-      </c>
-      <c r="E27" s="88" t="s">
-        <v>63</v>
       </c>
       <c r="F27" s="18">
         <f>(6.65+8)/0.75</f>
@@ -2429,43 +2426,43 @@
         <f>B27*G27</f>
         <v>21.877333333333336</v>
       </c>
-      <c r="I27" s="87" t="s">
-        <v>129</v>
-      </c>
-      <c r="J27" s="87" t="s">
-        <v>133</v>
-      </c>
-      <c r="K27" s="90" t="s">
+      <c r="I27" s="86" t="s">
         <v>128</v>
       </c>
-      <c r="L27" s="89" t="s">
+      <c r="J27" s="86" t="s">
+        <v>132</v>
+      </c>
+      <c r="K27" s="89" t="s">
+        <v>127</v>
+      </c>
+      <c r="L27" s="88" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="98" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="133"/>
-      <c r="B28" s="83"/>
-      <c r="C28" s="84"/>
-      <c r="D28" s="88"/>
-      <c r="E28" s="88"/>
+    <row r="28" spans="1:12" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="132"/>
+      <c r="B28" s="82"/>
+      <c r="C28" s="83"/>
+      <c r="D28" s="87"/>
+      <c r="E28" s="87"/>
       <c r="F28" s="18"/>
       <c r="G28" s="4"/>
       <c r="H28" s="16"/>
-      <c r="I28" s="97"/>
-      <c r="J28" s="89"/>
-    </row>
-    <row r="29" spans="1:12" s="98" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="133"/>
-      <c r="B29" s="96">
+      <c r="I28" s="96"/>
+      <c r="J28" s="88"/>
+    </row>
+    <row r="29" spans="1:12" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="132"/>
+      <c r="B29" s="95">
         <v>1</v>
       </c>
-      <c r="C29" s="84" t="s">
-        <v>142</v>
-      </c>
-      <c r="D29" s="88" t="s">
-        <v>90</v>
-      </c>
-      <c r="E29" s="101" t="s">
+      <c r="C29" s="83" t="s">
+        <v>141</v>
+      </c>
+      <c r="D29" s="87" t="s">
+        <v>89</v>
+      </c>
+      <c r="E29" s="100" t="s">
         <v>8</v>
       </c>
       <c r="F29" s="18">
@@ -2475,58 +2472,58 @@
         <f>F29*1.12</f>
         <v>11.200000000000001</v>
       </c>
-      <c r="H29" s="100">
+      <c r="H29" s="99">
         <f>B29*G29</f>
         <v>11.200000000000001</v>
       </c>
-      <c r="I29" s="102" t="s">
-        <v>91</v>
-      </c>
-      <c r="J29" s="89"/>
-    </row>
-    <row r="30" spans="1:12" s="95" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="134"/>
-      <c r="B30" s="77"/>
-      <c r="C30" s="92"/>
-      <c r="D30" s="99"/>
-      <c r="E30" s="99"/>
+      <c r="I29" s="101" t="s">
+        <v>90</v>
+      </c>
+      <c r="J29" s="88"/>
+    </row>
+    <row r="30" spans="1:12" s="94" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="133"/>
+      <c r="B30" s="76"/>
+      <c r="C30" s="91"/>
+      <c r="D30" s="98"/>
+      <c r="E30" s="98"/>
       <c r="F30" s="17"/>
-      <c r="G30" s="72"/>
-      <c r="H30" s="73"/>
-      <c r="I30" s="93"/>
-      <c r="J30" s="94" t="s">
+      <c r="G30" s="71"/>
+      <c r="H30" s="72"/>
+      <c r="I30" s="92"/>
+      <c r="J30" s="93" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="86" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="135" t="s">
+    <row r="31" spans="1:12" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="134" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="83"/>
-      <c r="C31" s="84"/>
-      <c r="D31" s="83"/>
-      <c r="E31" s="83"/>
+      <c r="B31" s="82"/>
+      <c r="C31" s="83"/>
+      <c r="D31" s="82"/>
+      <c r="E31" s="82"/>
       <c r="F31" s="16"/>
       <c r="G31" s="4"/>
       <c r="H31" s="16"/>
-      <c r="I31" s="85"/>
-      <c r="J31" s="89" t="s">
+      <c r="I31" s="84"/>
+      <c r="J31" s="88" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="86" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="136"/>
-      <c r="B32" s="83">
+    <row r="32" spans="1:12" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="135"/>
+      <c r="B32" s="82">
         <v>1</v>
       </c>
-      <c r="C32" s="84" t="s">
+      <c r="C32" s="83" t="s">
+        <v>130</v>
+      </c>
+      <c r="D32" s="87" t="s">
+        <v>48</v>
+      </c>
+      <c r="E32" s="87" t="s">
         <v>131</v>
-      </c>
-      <c r="D32" s="88" t="s">
-        <v>49</v>
-      </c>
-      <c r="E32" s="88" t="s">
-        <v>132</v>
       </c>
       <c r="F32" s="18">
         <v>15.99</v>
@@ -2539,26 +2536,26 @@
         <f t="shared" ref="H32" si="2">B32*G32</f>
         <v>17.908800000000003</v>
       </c>
-      <c r="I32" s="87" t="s">
-        <v>130</v>
-      </c>
-      <c r="J32" s="89" t="s">
+      <c r="I32" s="86" t="s">
+        <v>129</v>
+      </c>
+      <c r="J32" s="88" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="86" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="136"/>
-      <c r="B33" s="88" t="s">
-        <v>143</v>
-      </c>
-      <c r="C33" s="84" t="s">
-        <v>139</v>
-      </c>
-      <c r="D33" s="88" t="s">
-        <v>49</v>
-      </c>
-      <c r="E33" s="88" t="s">
-        <v>136</v>
+    <row r="33" spans="1:10" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="135"/>
+      <c r="B33" s="87" t="s">
+        <v>142</v>
+      </c>
+      <c r="C33" s="83" t="s">
+        <v>138</v>
+      </c>
+      <c r="D33" s="87" t="s">
+        <v>48</v>
+      </c>
+      <c r="E33" s="87" t="s">
+        <v>135</v>
       </c>
       <c r="F33" s="18">
         <v>12.99</v>
@@ -2571,26 +2568,26 @@
         <f>2*G33</f>
         <v>29.097600000000003</v>
       </c>
-      <c r="I33" s="87" t="s">
-        <v>135</v>
-      </c>
-      <c r="J33" s="89" t="s">
+      <c r="I33" s="86" t="s">
+        <v>134</v>
+      </c>
+      <c r="J33" s="88" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="86" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="136"/>
-      <c r="B34" s="83">
+    <row r="34" spans="1:10" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="135"/>
+      <c r="B34" s="82">
         <v>2</v>
       </c>
-      <c r="C34" s="84" t="s">
-        <v>140</v>
-      </c>
-      <c r="D34" s="88" t="s">
-        <v>49</v>
-      </c>
-      <c r="E34" s="88" t="s">
-        <v>80</v>
+      <c r="C34" s="83" t="s">
+        <v>139</v>
+      </c>
+      <c r="D34" s="87" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" s="87" t="s">
+        <v>79</v>
       </c>
       <c r="F34" s="18">
         <v>9.9499999999999993</v>
@@ -2603,26 +2600,26 @@
         <f t="shared" si="1"/>
         <v>22.288</v>
       </c>
-      <c r="I34" s="87" t="s">
-        <v>79</v>
-      </c>
-      <c r="J34" s="89" t="s">
+      <c r="I34" s="86" t="s">
+        <v>78</v>
+      </c>
+      <c r="J34" s="88" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="86" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="136"/>
-      <c r="B35" s="83">
+    <row r="35" spans="1:10" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="135"/>
+      <c r="B35" s="82">
         <v>2</v>
       </c>
-      <c r="C35" s="84" t="s">
-        <v>141</v>
-      </c>
-      <c r="D35" s="88" t="s">
-        <v>49</v>
-      </c>
-      <c r="E35" s="88" t="s">
-        <v>82</v>
+      <c r="C35" s="83" t="s">
+        <v>140</v>
+      </c>
+      <c r="D35" s="87" t="s">
+        <v>48</v>
+      </c>
+      <c r="E35" s="87" t="s">
+        <v>81</v>
       </c>
       <c r="F35" s="18">
         <v>10.43</v>
@@ -2635,26 +2632,26 @@
         <f t="shared" si="1"/>
         <v>23.363200000000003</v>
       </c>
-      <c r="I35" s="87" t="s">
-        <v>81</v>
-      </c>
-      <c r="J35" s="89" t="s">
+      <c r="I35" s="86" t="s">
+        <v>80</v>
+      </c>
+      <c r="J35" s="88" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="86" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="136"/>
-      <c r="B36" s="83">
+    <row r="36" spans="1:10" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="135"/>
+      <c r="B36" s="82">
         <v>1</v>
       </c>
-      <c r="C36" s="84" t="s">
-        <v>83</v>
-      </c>
-      <c r="D36" s="88" t="s">
-        <v>49</v>
-      </c>
-      <c r="E36" s="88" t="s">
-        <v>85</v>
+      <c r="C36" s="83" t="s">
+        <v>82</v>
+      </c>
+      <c r="D36" s="87" t="s">
+        <v>48</v>
+      </c>
+      <c r="E36" s="87" t="s">
+        <v>84</v>
       </c>
       <c r="F36" s="18">
         <v>9.99</v>
@@ -2667,40 +2664,40 @@
         <f t="shared" si="1"/>
         <v>11.188800000000001</v>
       </c>
-      <c r="I36" s="87" t="s">
-        <v>84</v>
-      </c>
-      <c r="J36" s="89" t="s">
+      <c r="I36" s="86" t="s">
+        <v>83</v>
+      </c>
+      <c r="J36" s="88" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="86" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="136"/>
-      <c r="B37" s="83"/>
-      <c r="C37" s="84"/>
-      <c r="D37" s="83"/>
-      <c r="E37" s="83"/>
+    <row r="37" spans="1:10" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="135"/>
+      <c r="B37" s="82"/>
+      <c r="C37" s="83"/>
+      <c r="D37" s="82"/>
+      <c r="E37" s="82"/>
       <c r="F37" s="18"/>
       <c r="G37" s="4"/>
       <c r="H37" s="16"/>
-      <c r="I37" s="85"/>
-      <c r="J37" s="89" t="s">
+      <c r="I37" s="84"/>
+      <c r="J37" s="88" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="86" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="136"/>
-      <c r="B38" s="83">
+    <row r="38" spans="1:10" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="135"/>
+      <c r="B38" s="82">
         <v>4</v>
       </c>
-      <c r="C38" s="84" t="s">
-        <v>89</v>
-      </c>
-      <c r="D38" s="88" t="s">
+      <c r="C38" s="83" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" s="87" t="s">
+        <v>86</v>
+      </c>
+      <c r="E38" s="87" t="s">
         <v>87</v>
-      </c>
-      <c r="E38" s="88" t="s">
-        <v>88</v>
       </c>
       <c r="F38" s="18">
         <v>1.6</v>
@@ -2713,55 +2710,55 @@
         <f t="shared" si="1"/>
         <v>7.168000000000001</v>
       </c>
-      <c r="I38" s="87" t="s">
-        <v>86</v>
-      </c>
-      <c r="J38" s="89" t="s">
+      <c r="I38" s="86" t="s">
+        <v>85</v>
+      </c>
+      <c r="J38" s="88" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="82" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="137"/>
-      <c r="B39" s="77"/>
-      <c r="C39" s="78"/>
-      <c r="D39" s="77"/>
-      <c r="E39" s="77"/>
-      <c r="F39" s="79"/>
-      <c r="G39" s="80"/>
-      <c r="H39" s="79"/>
-      <c r="I39" s="81"/>
-      <c r="J39" s="89" t="s">
+    <row r="39" spans="1:10" s="81" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="136"/>
+      <c r="B39" s="76"/>
+      <c r="C39" s="77"/>
+      <c r="D39" s="76"/>
+      <c r="E39" s="76"/>
+      <c r="F39" s="78"/>
+      <c r="G39" s="79"/>
+      <c r="H39" s="78"/>
+      <c r="I39" s="80"/>
+      <c r="J39" s="88" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="138" t="s">
+      <c r="A40" s="137" t="s">
         <v>11</v>
       </c>
       <c r="B40" s="3"/>
-      <c r="C40" s="119" t="s">
-        <v>120</v>
-      </c>
-      <c r="D40" s="70"/>
-      <c r="E40" s="70"/>
+      <c r="C40" s="118" t="s">
+        <v>119</v>
+      </c>
+      <c r="D40" s="69"/>
+      <c r="E40" s="69"/>
       <c r="F40" s="16"/>
       <c r="G40" s="4"/>
       <c r="H40" s="16"/>
       <c r="I40" s="23"/>
-      <c r="J40" s="89" t="s">
+      <c r="J40" s="88" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="139"/>
+      <c r="A41" s="138"/>
       <c r="B41" s="3">
         <v>1</v>
       </c>
-      <c r="C41" s="69" t="s">
-        <v>14</v>
-      </c>
-      <c r="D41" s="70"/>
-      <c r="E41" s="70"/>
+      <c r="C41" s="118" t="s">
+        <v>147</v>
+      </c>
+      <c r="D41" s="69"/>
+      <c r="E41" s="69"/>
       <c r="F41" s="18">
         <v>0</v>
       </c>
@@ -2774,20 +2771,20 @@
         <v>0</v>
       </c>
       <c r="I41" s="23"/>
-      <c r="J41" s="89" t="s">
+      <c r="J41" s="88" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="139"/>
+      <c r="A42" s="138"/>
       <c r="B42" s="3">
         <v>1</v>
       </c>
-      <c r="C42" s="119" t="s">
-        <v>114</v>
-      </c>
-      <c r="D42" s="70"/>
-      <c r="E42" s="70"/>
+      <c r="C42" s="118" t="s">
+        <v>113</v>
+      </c>
+      <c r="D42" s="69"/>
+      <c r="E42" s="69"/>
       <c r="F42" s="18">
         <v>0</v>
       </c>
@@ -2800,20 +2797,20 @@
         <v>0</v>
       </c>
       <c r="I42" s="23"/>
-      <c r="J42" s="89" t="s">
+      <c r="J42" s="88" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="139"/>
+      <c r="A43" s="138"/>
       <c r="B43" s="1">
         <v>1</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D43" s="70"/>
-      <c r="E43" s="70"/>
+        <v>14</v>
+      </c>
+      <c r="D43" s="69"/>
+      <c r="E43" s="69"/>
       <c r="F43" s="18">
         <v>0</v>
       </c>
@@ -2826,17 +2823,17 @@
         <v>0</v>
       </c>
       <c r="I43" s="23"/>
-      <c r="J43" s="89" t="s">
+      <c r="J43" s="88" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="139"/>
+      <c r="A44" s="138"/>
       <c r="B44" s="1">
         <v>1</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D44" s="13"/>
       <c r="E44" s="34"/>
@@ -2854,12 +2851,12 @@
       <c r="I44" s="23"/>
     </row>
     <row r="45" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="139"/>
+      <c r="A45" s="138"/>
       <c r="B45" s="1">
         <v>1</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D45" s="13"/>
       <c r="E45" s="34"/>
@@ -2877,12 +2874,12 @@
       <c r="I45" s="23"/>
     </row>
     <row r="46" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="139"/>
+      <c r="A46" s="138"/>
       <c r="B46" s="1">
         <v>1</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D46" s="13"/>
       <c r="E46" s="34"/>
@@ -2900,12 +2897,12 @@
       <c r="I46" s="24"/>
     </row>
     <row r="47" spans="1:10" s="52" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="139"/>
+      <c r="A47" s="138"/>
       <c r="B47" s="46">
         <v>1</v>
       </c>
       <c r="C47" s="47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D47" s="46"/>
       <c r="E47" s="48"/>
@@ -2923,12 +2920,12 @@
       <c r="I47" s="51"/>
     </row>
     <row r="48" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="139"/>
+      <c r="A48" s="138"/>
       <c r="B48" s="1">
         <v>1</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D48" s="13"/>
       <c r="E48" s="34"/>
@@ -2946,12 +2943,12 @@
       <c r="I48" s="24"/>
     </row>
     <row r="49" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="139"/>
+      <c r="A49" s="138"/>
       <c r="B49" s="1">
         <v>1</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D49" s="13"/>
       <c r="E49" s="34"/>
@@ -2969,12 +2966,12 @@
       <c r="I49" s="21"/>
     </row>
     <row r="50" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="139"/>
+      <c r="A50" s="138"/>
       <c r="B50" s="1">
         <v>1</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D50" s="13"/>
       <c r="E50" s="34"/>
@@ -2992,12 +2989,12 @@
       <c r="I50" s="24"/>
     </row>
     <row r="51" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="139"/>
+      <c r="A51" s="138"/>
       <c r="B51" s="22">
         <v>1</v>
       </c>
       <c r="C51" s="32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D51" s="13"/>
       <c r="E51" s="35"/>
@@ -3015,12 +3012,12 @@
       <c r="I51" s="36"/>
     </row>
     <row r="52" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="139"/>
+      <c r="A52" s="138"/>
       <c r="B52" s="22">
         <v>1</v>
       </c>
       <c r="C52" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D52" s="13"/>
       <c r="E52" s="35"/>
@@ -3038,12 +3035,12 @@
       <c r="I52" s="36"/>
     </row>
     <row r="53" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="139"/>
+      <c r="A53" s="138"/>
       <c r="B53" s="22">
         <v>1</v>
       </c>
       <c r="C53" s="32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D53" s="13"/>
       <c r="E53" s="35"/>
@@ -3061,12 +3058,12 @@
       <c r="I53" s="36"/>
     </row>
     <row r="54" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="139"/>
+      <c r="A54" s="138"/>
       <c r="B54" s="22">
         <v>1</v>
       </c>
       <c r="C54" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D54" s="13"/>
       <c r="E54" s="35"/>
@@ -3084,12 +3081,12 @@
       <c r="I54" s="36"/>
     </row>
     <row r="55" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="139"/>
+      <c r="A55" s="138"/>
       <c r="B55" s="22">
         <v>1</v>
       </c>
       <c r="C55" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D55" s="27"/>
       <c r="E55" s="35"/>
@@ -3107,12 +3104,12 @@
       <c r="I55" s="33"/>
     </row>
     <row r="56" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="139"/>
+      <c r="A56" s="138"/>
       <c r="B56" s="22">
         <v>1</v>
       </c>
       <c r="C56" s="32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D56" s="37"/>
       <c r="E56" s="35"/>
@@ -3130,12 +3127,12 @@
       <c r="I56" s="33"/>
     </row>
     <row r="57" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="139"/>
+      <c r="A57" s="138"/>
       <c r="B57" s="22">
         <v>1</v>
       </c>
       <c r="C57" s="32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D57" s="13"/>
       <c r="E57" s="34"/>
@@ -3153,12 +3150,12 @@
       <c r="I57" s="24"/>
     </row>
     <row r="58" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="139"/>
+      <c r="A58" s="138"/>
       <c r="B58" s="22">
         <v>1</v>
       </c>
       <c r="C58" s="32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D58" s="27"/>
       <c r="E58" s="35"/>
@@ -3176,12 +3173,12 @@
       <c r="I58" s="42"/>
     </row>
     <row r="59" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="139"/>
+      <c r="A59" s="138"/>
       <c r="B59" s="22">
         <v>1</v>
       </c>
       <c r="C59" s="32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D59" s="37"/>
       <c r="E59" s="35"/>
@@ -3199,12 +3196,12 @@
       <c r="I59" s="42"/>
     </row>
     <row r="60" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="139"/>
+      <c r="A60" s="138"/>
       <c r="B60" s="22">
         <v>1</v>
       </c>
       <c r="C60" s="32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D60" s="37"/>
       <c r="E60" s="35"/>
@@ -3222,12 +3219,12 @@
       <c r="I60" s="33"/>
     </row>
     <row r="61" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="139"/>
+      <c r="A61" s="138"/>
       <c r="B61" s="22">
         <v>1</v>
       </c>
       <c r="C61" s="32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D61" s="37"/>
       <c r="E61" s="35"/>
@@ -3245,12 +3242,12 @@
       <c r="I61" s="33"/>
     </row>
     <row r="62" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="139"/>
+      <c r="A62" s="138"/>
       <c r="B62" s="22">
         <v>1</v>
       </c>
       <c r="C62" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D62" s="37"/>
       <c r="E62" s="35"/>
@@ -3268,12 +3265,12 @@
       <c r="I62" s="33"/>
     </row>
     <row r="63" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="139"/>
+      <c r="A63" s="138"/>
       <c r="B63" s="22">
         <v>1</v>
       </c>
       <c r="C63" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D63" s="37"/>
       <c r="E63" s="35"/>
@@ -3291,12 +3288,12 @@
       <c r="I63" s="33"/>
     </row>
     <row r="64" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="139"/>
+      <c r="A64" s="138"/>
       <c r="B64" s="22">
         <v>1</v>
       </c>
       <c r="C64" s="32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D64" s="37"/>
       <c r="E64" s="35"/>
@@ -3314,65 +3311,65 @@
       <c r="I64" s="33"/>
     </row>
     <row r="65" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="139"/>
+      <c r="A65" s="138"/>
       <c r="B65" s="22">
         <v>1</v>
       </c>
-      <c r="C65" s="117" t="s">
-        <v>37</v>
+      <c r="C65" s="116" t="s">
+        <v>36</v>
       </c>
       <c r="D65" s="37"/>
       <c r="E65" s="35"/>
-      <c r="F65" s="147">
-        <v>0</v>
-      </c>
-      <c r="G65" s="150">
+      <c r="F65" s="146">
+        <v>0</v>
+      </c>
+      <c r="G65" s="149">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="H65" s="147">
+      <c r="H65" s="146">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I65" s="33"/>
     </row>
     <row r="66" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="139"/>
+      <c r="A66" s="138"/>
       <c r="B66" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="C66" s="116" t="s">
         <v>125</v>
-      </c>
-      <c r="C66" s="117" t="s">
-        <v>126</v>
       </c>
       <c r="D66" s="37"/>
       <c r="E66" s="35"/>
-      <c r="F66" s="148"/>
-      <c r="G66" s="151"/>
-      <c r="H66" s="148"/>
+      <c r="F66" s="147"/>
+      <c r="G66" s="150"/>
+      <c r="H66" s="147"/>
       <c r="I66" s="33"/>
     </row>
     <row r="67" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="139"/>
+      <c r="A67" s="138"/>
       <c r="B67" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="C67" s="117" t="s">
-        <v>127</v>
+        <v>124</v>
+      </c>
+      <c r="C67" s="116" t="s">
+        <v>126</v>
       </c>
       <c r="D67" s="37"/>
       <c r="E67" s="35"/>
-      <c r="F67" s="149"/>
-      <c r="G67" s="152"/>
-      <c r="H67" s="149"/>
+      <c r="F67" s="148"/>
+      <c r="G67" s="151"/>
+      <c r="H67" s="148"/>
       <c r="I67" s="33"/>
     </row>
     <row r="68" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="139"/>
+      <c r="A68" s="138"/>
       <c r="B68" s="22">
         <v>1</v>
       </c>
       <c r="C68" s="32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D68" s="37"/>
       <c r="E68" s="35"/>
@@ -3390,12 +3387,12 @@
       <c r="I68" s="33"/>
     </row>
     <row r="69" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="139"/>
+      <c r="A69" s="138"/>
       <c r="B69" s="22">
         <v>1</v>
       </c>
-      <c r="C69" s="117" t="s">
-        <v>115</v>
+      <c r="C69" s="116" t="s">
+        <v>114</v>
       </c>
       <c r="D69" s="37"/>
       <c r="E69" s="35"/>
@@ -3413,12 +3410,12 @@
       <c r="I69" s="33"/>
     </row>
     <row r="70" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="139"/>
+      <c r="A70" s="138"/>
       <c r="B70" s="22">
         <v>1</v>
       </c>
-      <c r="C70" s="117" t="s">
-        <v>122</v>
+      <c r="C70" s="116" t="s">
+        <v>121</v>
       </c>
       <c r="D70" s="37"/>
       <c r="E70" s="35"/>
@@ -3436,12 +3433,12 @@
       <c r="I70" s="33"/>
     </row>
     <row r="71" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="139"/>
+      <c r="A71" s="138"/>
       <c r="B71" s="22">
         <v>1</v>
       </c>
       <c r="C71" s="32" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D71" s="37"/>
       <c r="E71" s="35"/>
@@ -3459,12 +3456,12 @@
       <c r="I71" s="33"/>
     </row>
     <row r="72" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="139"/>
+      <c r="A72" s="138"/>
       <c r="B72" s="22">
         <v>1</v>
       </c>
       <c r="C72" s="32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D72" s="37"/>
       <c r="E72" s="35"/>
@@ -3482,12 +3479,12 @@
       <c r="I72" s="33"/>
     </row>
     <row r="73" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="139"/>
+      <c r="A73" s="138"/>
       <c r="B73" s="22">
         <v>1</v>
       </c>
       <c r="C73" s="32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D73" s="37"/>
       <c r="E73" s="35"/>
@@ -3505,12 +3502,12 @@
       <c r="I73" s="33"/>
     </row>
     <row r="74" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="139"/>
+      <c r="A74" s="138"/>
       <c r="B74" s="22">
         <v>1</v>
       </c>
       <c r="C74" s="32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D74" s="37"/>
       <c r="E74" s="35"/>
@@ -3528,12 +3525,12 @@
       <c r="I74" s="33"/>
     </row>
     <row r="75" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="139"/>
+      <c r="A75" s="138"/>
       <c r="B75" s="22">
         <v>1</v>
       </c>
       <c r="C75" s="32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D75" s="37"/>
       <c r="E75" s="35"/>
@@ -3551,12 +3548,12 @@
       <c r="I75" s="33"/>
     </row>
     <row r="76" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="139"/>
+      <c r="A76" s="138"/>
       <c r="B76" s="22">
         <v>1</v>
       </c>
       <c r="C76" s="32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D76" s="37"/>
       <c r="E76" s="35"/>
@@ -3574,12 +3571,12 @@
       <c r="I76" s="33"/>
     </row>
     <row r="77" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="139"/>
+      <c r="A77" s="138"/>
       <c r="B77" s="22">
         <v>1</v>
       </c>
       <c r="C77" s="32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D77" s="37"/>
       <c r="E77" s="35"/>
@@ -3597,12 +3594,12 @@
       <c r="I77" s="33"/>
     </row>
     <row r="78" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="139"/>
+      <c r="A78" s="138"/>
       <c r="B78" s="22">
         <v>1</v>
       </c>
-      <c r="C78" s="117" t="s">
-        <v>138</v>
+      <c r="C78" s="116" t="s">
+        <v>137</v>
       </c>
       <c r="D78" s="37"/>
       <c r="E78" s="35"/>
@@ -3620,12 +3617,12 @@
       <c r="I78" s="33"/>
     </row>
     <row r="79" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="139"/>
+      <c r="A79" s="138"/>
       <c r="B79" s="22">
         <v>1</v>
       </c>
-      <c r="C79" s="117" t="s">
-        <v>116</v>
+      <c r="C79" s="116" t="s">
+        <v>115</v>
       </c>
       <c r="D79" s="37"/>
       <c r="E79" s="35"/>
@@ -3643,12 +3640,12 @@
       <c r="I79" s="33"/>
     </row>
     <row r="80" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="139"/>
+      <c r="A80" s="138"/>
       <c r="B80" s="22">
         <v>1</v>
       </c>
-      <c r="C80" s="117" t="s">
-        <v>137</v>
+      <c r="C80" s="116" t="s">
+        <v>136</v>
       </c>
       <c r="D80" s="37"/>
       <c r="E80" s="35"/>
@@ -3666,12 +3663,12 @@
       <c r="I80" s="33"/>
     </row>
     <row r="81" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="139"/>
+      <c r="A81" s="138"/>
       <c r="B81" s="22">
         <v>1</v>
       </c>
-      <c r="C81" s="117" t="s">
-        <v>45</v>
+      <c r="C81" s="116" t="s">
+        <v>44</v>
       </c>
       <c r="D81" s="37"/>
       <c r="E81" s="35"/>
@@ -3689,12 +3686,12 @@
       <c r="I81" s="33"/>
     </row>
     <row r="82" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="139"/>
+      <c r="A82" s="138"/>
       <c r="B82" s="22">
         <v>1</v>
       </c>
-      <c r="C82" s="117" t="s">
-        <v>113</v>
+      <c r="C82" s="116" t="s">
+        <v>112</v>
       </c>
       <c r="D82" s="37"/>
       <c r="E82" s="35"/>
@@ -3712,12 +3709,12 @@
       <c r="I82" s="33"/>
     </row>
     <row r="83" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="139"/>
+      <c r="A83" s="138"/>
       <c r="B83" s="22">
         <v>1</v>
       </c>
       <c r="C83" s="32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D83" s="37"/>
       <c r="E83" s="35"/>
@@ -3735,12 +3732,12 @@
       <c r="I83" s="33"/>
     </row>
     <row r="84" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="139"/>
+      <c r="A84" s="138"/>
       <c r="B84" s="22">
         <v>1</v>
       </c>
       <c r="C84" s="32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D84" s="37"/>
       <c r="E84" s="35"/>
@@ -3758,66 +3755,66 @@
       <c r="I84" s="33"/>
     </row>
     <row r="85" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="139"/>
-      <c r="B85" s="120"/>
+      <c r="A85" s="138"/>
+      <c r="B85" s="119"/>
       <c r="C85" s="54"/>
-      <c r="D85" s="121"/>
+      <c r="D85" s="120"/>
       <c r="E85" s="56"/>
-      <c r="F85" s="122"/>
-      <c r="G85" s="123"/>
-      <c r="H85" s="124"/>
-      <c r="I85" s="125"/>
+      <c r="F85" s="121"/>
+      <c r="G85" s="122"/>
+      <c r="H85" s="123"/>
+      <c r="I85" s="124"/>
     </row>
     <row r="86" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="139"/>
-      <c r="B86" s="144" t="s">
-        <v>110</v>
-      </c>
-      <c r="C86" s="145"/>
-      <c r="D86" s="145"/>
-      <c r="E86" s="145"/>
-      <c r="F86" s="145"/>
-      <c r="G86" s="145"/>
-      <c r="H86" s="145"/>
-      <c r="I86" s="146"/>
+      <c r="A86" s="138"/>
+      <c r="B86" s="143" t="s">
+        <v>109</v>
+      </c>
+      <c r="C86" s="144"/>
+      <c r="D86" s="144"/>
+      <c r="E86" s="144"/>
+      <c r="F86" s="144"/>
+      <c r="G86" s="144"/>
+      <c r="H86" s="144"/>
+      <c r="I86" s="145"/>
     </row>
     <row r="87" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="139"/>
+      <c r="A87" s="138"/>
       <c r="B87" s="22">
         <v>1</v>
       </c>
-      <c r="C87" s="118" t="s">
-        <v>109</v>
+      <c r="C87" s="117" t="s">
+        <v>108</v>
       </c>
       <c r="D87" s="54"/>
       <c r="E87" s="54"/>
-      <c r="F87" s="114"/>
-      <c r="G87" s="115"/>
-      <c r="H87" s="115"/>
-      <c r="I87" s="116"/>
+      <c r="F87" s="113"/>
+      <c r="G87" s="114"/>
+      <c r="H87" s="114"/>
+      <c r="I87" s="115"/>
     </row>
     <row r="88" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="139"/>
+      <c r="A88" s="138"/>
       <c r="B88" s="22">
         <v>1</v>
       </c>
-      <c r="C88" s="118" t="s">
-        <v>111</v>
+      <c r="C88" s="117" t="s">
+        <v>110</v>
       </c>
       <c r="D88" s="54"/>
       <c r="E88" s="54"/>
-      <c r="F88" s="114"/>
-      <c r="G88" s="115"/>
-      <c r="H88" s="115"/>
-      <c r="I88" s="116"/>
+      <c r="F88" s="113"/>
+      <c r="G88" s="114"/>
+      <c r="H88" s="114"/>
+      <c r="I88" s="115"/>
     </row>
     <row r="89" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="139"/>
+      <c r="A89" s="138"/>
       <c r="B89" s="22">
         <v>1</v>
       </c>
-      <c r="C89" s="117" t="s">
-        <v>112</v>
+      <c r="C89" s="116" t="s">
+        <v>111</v>
       </c>
       <c r="D89" s="37"/>
       <c r="E89" s="35"/>
@@ -3827,12 +3824,12 @@
       <c r="I89" s="33"/>
     </row>
     <row r="90" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="139"/>
+      <c r="A90" s="138"/>
       <c r="B90" s="22">
         <v>1</v>
       </c>
-      <c r="C90" s="117" t="s">
-        <v>101</v>
+      <c r="C90" s="116" t="s">
+        <v>100</v>
       </c>
       <c r="D90" s="37"/>
       <c r="E90" s="35"/>
@@ -3850,12 +3847,12 @@
       <c r="I90" s="33"/>
     </row>
     <row r="91" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="139"/>
+      <c r="A91" s="138"/>
       <c r="B91" s="22">
         <v>1</v>
       </c>
-      <c r="C91" s="117" t="s">
-        <v>102</v>
+      <c r="C91" s="116" t="s">
+        <v>101</v>
       </c>
       <c r="D91" s="37"/>
       <c r="E91" s="35"/>
@@ -3873,12 +3870,12 @@
       <c r="I91" s="33"/>
     </row>
     <row r="92" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="139"/>
+      <c r="A92" s="138"/>
       <c r="B92" s="22">
         <v>1</v>
       </c>
-      <c r="C92" s="117" t="s">
-        <v>103</v>
+      <c r="C92" s="116" t="s">
+        <v>102</v>
       </c>
       <c r="D92" s="37"/>
       <c r="E92" s="35"/>
@@ -3896,12 +3893,12 @@
       <c r="I92" s="33"/>
     </row>
     <row r="93" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="139"/>
+      <c r="A93" s="138"/>
       <c r="B93" s="22">
         <v>1</v>
       </c>
-      <c r="C93" s="117" t="s">
-        <v>104</v>
+      <c r="C93" s="116" t="s">
+        <v>103</v>
       </c>
       <c r="D93" s="37"/>
       <c r="E93" s="35"/>
@@ -3919,12 +3916,12 @@
       <c r="I93" s="33"/>
     </row>
     <row r="94" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="139"/>
+      <c r="A94" s="138"/>
       <c r="B94" s="22">
         <v>1</v>
       </c>
-      <c r="C94" s="117" t="s">
-        <v>105</v>
+      <c r="C94" s="116" t="s">
+        <v>104</v>
       </c>
       <c r="D94" s="37"/>
       <c r="E94" s="35"/>
@@ -3942,12 +3939,12 @@
       <c r="I94" s="33"/>
     </row>
     <row r="95" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="139"/>
+      <c r="A95" s="138"/>
       <c r="B95" s="22">
         <v>1</v>
       </c>
-      <c r="C95" s="117" t="s">
-        <v>106</v>
+      <c r="C95" s="116" t="s">
+        <v>105</v>
       </c>
       <c r="D95" s="37"/>
       <c r="E95" s="35"/>
@@ -3965,12 +3962,12 @@
       <c r="I95" s="33"/>
     </row>
     <row r="96" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="139"/>
+      <c r="A96" s="138"/>
       <c r="B96" s="22">
         <v>1</v>
       </c>
-      <c r="C96" s="117" t="s">
-        <v>108</v>
+      <c r="C96" s="116" t="s">
+        <v>107</v>
       </c>
       <c r="D96" s="37"/>
       <c r="E96" s="35"/>
@@ -3988,12 +3985,12 @@
       <c r="I96" s="33"/>
     </row>
     <row r="97" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="139"/>
+      <c r="A97" s="138"/>
       <c r="B97" s="22">
         <v>1</v>
       </c>
-      <c r="C97" s="117" t="s">
-        <v>107</v>
+      <c r="C97" s="116" t="s">
+        <v>106</v>
       </c>
       <c r="D97" s="37"/>
       <c r="E97" s="35"/>
@@ -4011,12 +4008,12 @@
       <c r="I97" s="33"/>
     </row>
     <row r="98" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="139"/>
+      <c r="A98" s="138"/>
       <c r="B98" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="C98" s="117" t="s">
         <v>118</v>
+      </c>
+      <c r="C98" s="116" t="s">
+        <v>117</v>
       </c>
       <c r="D98" s="37"/>
       <c r="E98" s="35"/>
@@ -4033,12 +4030,12 @@
       <c r="I98" s="33"/>
     </row>
     <row r="99" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="139"/>
+      <c r="A99" s="138"/>
       <c r="B99" s="22">
         <v>1</v>
       </c>
-      <c r="C99" s="117" t="s">
-        <v>117</v>
+      <c r="C99" s="116" t="s">
+        <v>116</v>
       </c>
       <c r="D99" s="37"/>
       <c r="E99" s="35"/>
@@ -4056,7 +4053,7 @@
       <c r="I99" s="33"/>
     </row>
     <row r="100" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="140"/>
+      <c r="A100" s="139"/>
       <c r="B100" s="8"/>
       <c r="C100" s="12"/>
       <c r="D100" s="29"/>
@@ -4607,13 +4604,13 @@
     </row>
     <row r="150" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="61"/>
-      <c r="B150" s="126"/>
-      <c r="C150" s="126"/>
-      <c r="D150" s="126"/>
-      <c r="E150" s="126"/>
-      <c r="F150" s="126"/>
-      <c r="G150" s="126"/>
-      <c r="H150" s="127"/>
+      <c r="B150" s="125"/>
+      <c r="C150" s="125"/>
+      <c r="D150" s="125"/>
+      <c r="E150" s="125"/>
+      <c r="F150" s="125"/>
+      <c r="G150" s="125"/>
+      <c r="H150" s="126"/>
       <c r="I150" s="40"/>
     </row>
     <row r="151" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated to power supply description and link
</commit_message>
<xml_diff>
--- a/TurbofanDriver - V3 Bill of Materials.xlsx
+++ b/TurbofanDriver - V3 Bill of Materials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/844add23945bcd8f/Documents/3D Printer Shit/1___3D_Printable_Jet_Engine_Upgrade/V3 Upgrades/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="892" documentId="13_ncr:1_{2F400004-E652-4E60-AF98-6B4D8D866B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB678AD8-09DE-46D7-8513-BCDCFD419D9C}"/>
+  <xr:revisionPtr revIDLastSave="898" documentId="13_ncr:1_{2F400004-E652-4E60-AF98-6B4D8D866B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8359D035-3AC9-4233-86A6-BEF8C5A92856}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5160" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials - Rev 1" sheetId="3" r:id="rId1"/>
@@ -524,16 +524,16 @@
     <t>4A Rated Latching Push Button Switch 1NO1NC SPDT (or 1NO SPST) Black Metal Shell with Blue LED for 19mm 3/4"</t>
   </si>
   <si>
-    <t>https://www.amazon.ca/gp/product/B09BQBWKKT/?th=1</t>
+    <t>Electronics_Bay_Cover_-_V3</t>
   </si>
   <si>
-    <t>12V ≥4A Power Supply, AC Adapter 100-240V 50-60hz (&lt; 125mm long, 55mm wide, 34mm tall)</t>
+    <t>12V ≥4A Power Supply, AC Adapter 100-240V 50-60hz (&lt; 125mm long, 55mm wide, 35mm tall)</t>
   </si>
   <si>
-    <t>B09BQBWKKT</t>
+    <t>https://www.amazon.ca/gp/product/B01GEA8PQA/?th=1</t>
   </si>
   <si>
-    <t>Electronics_Bay_Cover_-_V3</t>
+    <t>B01GEA8PQA</t>
   </si>
 </sst>
 </file>
@@ -1786,10 +1786,10 @@
   <dimension ref="A1:L1077"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C43" sqref="C43"/>
+      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1870,7 +1870,7 @@
       </c>
       <c r="H5" s="127">
         <f xml:space="preserve"> H7+H9</f>
-        <v>370.83573333333339</v>
+        <v>366.35573333333338</v>
       </c>
       <c r="I5" s="108"/>
       <c r="J5" s="88" t="s">
@@ -1905,7 +1905,7 @@
       </c>
       <c r="H7" s="106">
         <f>SUM(H14:H29)</f>
-        <v>259.82133333333337</v>
+        <v>255.34133333333335</v>
       </c>
       <c r="I7" s="104"/>
     </row>
@@ -2285,21 +2285,21 @@
         <v>48</v>
       </c>
       <c r="E22" s="87" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F22" s="18">
-        <v>21.99</v>
+        <v>17.989999999999998</v>
       </c>
       <c r="G22" s="4">
         <f t="shared" si="0"/>
-        <v>24.628800000000002</v>
+        <v>20.148800000000001</v>
       </c>
       <c r="H22" s="16">
         <f t="shared" si="1"/>
-        <v>24.628800000000002</v>
+        <v>20.148800000000001</v>
       </c>
       <c r="I22" s="86" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="J22" s="88" t="s">
         <v>8</v>
@@ -2755,7 +2755,7 @@
         <v>1</v>
       </c>
       <c r="C41" s="118" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D41" s="69"/>
       <c r="E41" s="69"/>
@@ -14838,7 +14838,7 @@
     <hyperlink ref="K25" r:id="rId16" xr:uid="{4896C6AA-E74F-4FD2-94AF-03164218594A}"/>
     <hyperlink ref="K27" r:id="rId17" xr:uid="{5304B522-7BFB-4401-9BB1-C7AF779A47B6}"/>
     <hyperlink ref="J27" r:id="rId18" xr:uid="{DA1BC955-C30B-42D2-8DF9-55540D3C26E8}"/>
-    <hyperlink ref="I22" r:id="rId19" xr:uid="{2456F480-71EF-4AD3-A93F-EA30D00CD933}"/>
+    <hyperlink ref="I22" r:id="rId19" xr:uid="{DAE7766D-F4DD-40D5-87EC-5035F7AAC8E9}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Update to bearings, and kit cost
Updated bearings to sealed/lubricated type and updated mechanical kit cost
</commit_message>
<xml_diff>
--- a/TurbofanDriver - V3 Bill of Materials.xlsx
+++ b/TurbofanDriver - V3 Bill of Materials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/844add23945bcd8f/Documents/3D Printer Shit/1___3D_Printable_Jet_Engine_Upgrade/V3 Upgrades/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="898" documentId="13_ncr:1_{2F400004-E652-4E60-AF98-6B4D8D866B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8359D035-3AC9-4233-86A6-BEF8C5A92856}"/>
+  <xr:revisionPtr revIDLastSave="929" documentId="13_ncr:1_{2F400004-E652-4E60-AF98-6B4D8D866B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C89CA6BE-CAE5-495A-92B8-5D365BECAC0F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="5160" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials - Rev 1" sheetId="3" r:id="rId1"/>
@@ -267,18 +267,6 @@
     <t>COTS Electronics</t>
   </si>
   <si>
-    <t>https://www.amazon.com/6204-Bearing-20x47x14-Open-Bearings/dp/B00IK4MCC2/</t>
-  </si>
-  <si>
-    <t>B00IK4MCC2</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/6003-Bearing-Deep-Groove-Bearings/dp/B00FNU80CC</t>
-  </si>
-  <si>
-    <t>B00FNU80CC</t>
-  </si>
-  <si>
     <t>Gorilla Glue Super Glue Gel, Cyanoacrylate Glue, Clear, 0.71oz/20g, (Pack of 1)</t>
   </si>
   <si>
@@ -328,48 +316,6 @@
   </si>
   <si>
     <t>https://www.amazon.ca/gp/product/B0CBRGQGFS/</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Turbofan Driver - Bill of Materials</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>V3 Upgrade, 17 August 2024                                                                                                                      (https://github.com/nairck/TurbofanDriver       https://www.thingiverse.com/thing:4743929)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Created by Adam B. Johnson</t>
-    </r>
   </si>
   <si>
     <t>TN1-118A_TFD-V3</t>
@@ -509,12 +455,6 @@
     <t>M3x0.5, 8mm Length, Button Head Hex Socket Drive Screws (2 Packs of 100)</t>
   </si>
   <si>
-    <t>6204 Size Ball Bearing, Open, Sealed/Lubricated, or Shielded/Lubricated, 20x47x14 mm</t>
-  </si>
-  <si>
-    <t>6003 Size Ball Bearing, Open, Sealed, or Shielded, 17x35x10 mm</t>
-  </si>
-  <si>
     <t>Driver Board PCB by Cyberfox361 (Upload Gerber files (ZIP file) jlcpcb.com to order)</t>
   </si>
   <si>
@@ -534,6 +474,66 @@
   </si>
   <si>
     <t>B01GEA8PQA</t>
+  </si>
+  <si>
+    <t>https://www.amazon.ca/PGN-6003-2RS-Sealed-Ball-Bearing/dp/B07GVPRWG6/</t>
+  </si>
+  <si>
+    <t>B07GVPRWG6</t>
+  </si>
+  <si>
+    <t>6003 Size Ball Bearing, Sealed/Lubricated, Shielded, or Open, 17x35x10 mm (Pack of 2)</t>
+  </si>
+  <si>
+    <t>6204 Size Ball Bearing, Sealed/Lubricated, Shielded, or Open, 20x47x14 mm (Pack of 2)</t>
+  </si>
+  <si>
+    <t>https://www.amazon.ca/MAPLE-ACE-6204-2RS-Bearing-20x47x14mm/dp/B0971X5QJT/?th=1</t>
+  </si>
+  <si>
+    <t>B0971X5QJT</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Turbofan Driver - Bill of Materials</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>V3 Upgrade, Aug-Sep 2024                                                                                                                      (https://github.com/nairck/TurbofanDriver       https://www.thingiverse.com/thing:4743929)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Created by Adam B. Johnson</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1786,10 +1786,10 @@
   <dimension ref="A1:L1077"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1806,7 +1806,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="129" t="s">
-        <v>99</v>
+        <v>147</v>
       </c>
       <c r="C1" s="129"/>
       <c r="D1" s="129"/>
@@ -1845,7 +1845,7 @@
       </c>
       <c r="C4" s="107"/>
       <c r="G4" s="107" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="H4" s="110" t="s">
         <v>5</v>
@@ -1860,17 +1860,17 @@
         <v>1</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="127">
-        <v>250</v>
+        <v>225</v>
       </c>
       <c r="H5" s="127">
         <f xml:space="preserve"> H7+H9</f>
-        <v>366.35573333333338</v>
+        <v>346.80053333333336</v>
       </c>
       <c r="I5" s="108"/>
       <c r="J5" s="88" t="s">
@@ -1880,7 +1880,7 @@
     <row r="6" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="141"/>
       <c r="C6" s="11" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D6" s="28"/>
       <c r="E6" s="3"/>
@@ -1905,7 +1905,7 @@
       </c>
       <c r="H7" s="106">
         <f>SUM(H14:H29)</f>
-        <v>255.34133333333335</v>
+        <v>249.59573333333336</v>
       </c>
       <c r="I7" s="104"/>
     </row>
@@ -1913,7 +1913,7 @@
       <c r="A8" s="141"/>
       <c r="B8" s="1"/>
       <c r="C8" s="11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="34"/>
@@ -1942,7 +1942,7 @@
       </c>
       <c r="H9" s="103">
         <f>SUM(H32:H38)</f>
-        <v>111.01440000000002</v>
+        <v>97.20480000000002</v>
       </c>
       <c r="I9" s="104"/>
     </row>
@@ -1950,13 +1950,13 @@
       <c r="A10" s="141"/>
       <c r="B10" s="1"/>
       <c r="C10" s="11" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="34"/>
       <c r="F10" s="34"/>
       <c r="G10" s="102">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="H10" s="102">
         <v>0</v>
@@ -1999,10 +1999,10 @@
         <v>10</v>
       </c>
       <c r="J12" s="107" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K12" s="107" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="85" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -2087,7 +2087,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="83" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D16" s="87" t="s">
         <v>48</v>
@@ -2119,13 +2119,13 @@
         <v>1</v>
       </c>
       <c r="C17" s="83" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D17" s="87" t="s">
         <v>48</v>
       </c>
       <c r="E17" s="87" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F17" s="18">
         <v>13.99</v>
@@ -2139,7 +2139,7 @@
         <v>15.668800000000001</v>
       </c>
       <c r="I17" s="86" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="J17" s="88" t="s">
         <v>8</v>
@@ -2279,13 +2279,13 @@
         <v>1</v>
       </c>
       <c r="C22" s="83" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D22" s="87" t="s">
         <v>48</v>
       </c>
       <c r="E22" s="87" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="F22" s="18">
         <v>17.989999999999998</v>
@@ -2299,7 +2299,7 @@
         <v>20.148800000000001</v>
       </c>
       <c r="I22" s="86" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="J22" s="88" t="s">
         <v>8</v>
@@ -2355,7 +2355,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="83" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D25" s="87" t="s">
         <v>59</v>
@@ -2382,7 +2382,7 @@
         <v>8</v>
       </c>
       <c r="K25" s="89" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="L25" s="88" t="s">
         <v>8</v>
@@ -2427,13 +2427,13 @@
         <v>21.877333333333336</v>
       </c>
       <c r="I27" s="86" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="J27" s="86" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="K27" s="89" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="L27" s="88" t="s">
         <v>8</v>
@@ -2457,27 +2457,27 @@
         <v>1</v>
       </c>
       <c r="C29" s="83" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D29" s="87" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E29" s="100" t="s">
         <v>8</v>
       </c>
       <c r="F29" s="18">
-        <v>10</v>
+        <v>4.87</v>
       </c>
       <c r="G29" s="4">
         <f>F29*1.12</f>
-        <v>11.200000000000001</v>
+        <v>5.4544000000000006</v>
       </c>
       <c r="H29" s="99">
         <f>B29*G29</f>
-        <v>11.200000000000001</v>
+        <v>5.4544000000000006</v>
       </c>
       <c r="I29" s="101" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J29" s="88"/>
     </row>
@@ -2517,13 +2517,13 @@
         <v>1</v>
       </c>
       <c r="C32" s="83" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D32" s="87" t="s">
         <v>48</v>
       </c>
       <c r="E32" s="87" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F32" s="18">
         <v>15.99</v>
@@ -2537,7 +2537,7 @@
         <v>17.908800000000003</v>
       </c>
       <c r="I32" s="86" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="J32" s="88" t="s">
         <v>8</v>
@@ -2546,16 +2546,16 @@
     <row r="33" spans="1:10" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="135"/>
       <c r="B33" s="87" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C33" s="83" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D33" s="87" t="s">
         <v>48</v>
       </c>
       <c r="E33" s="87" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F33" s="18">
         <v>12.99</v>
@@ -2569,7 +2569,7 @@
         <v>29.097600000000003</v>
       </c>
       <c r="I33" s="86" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="J33" s="88" t="s">
         <v>8</v>
@@ -2578,30 +2578,30 @@
     <row r="34" spans="1:10" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="135"/>
       <c r="B34" s="82">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C34" s="83" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="D34" s="87" t="s">
         <v>48</v>
       </c>
       <c r="E34" s="87" t="s">
-        <v>79</v>
+        <v>146</v>
       </c>
       <c r="F34" s="18">
-        <v>9.9499999999999993</v>
+        <v>13.35</v>
       </c>
       <c r="G34" s="4">
         <f t="shared" si="0"/>
-        <v>11.144</v>
+        <v>14.952000000000002</v>
       </c>
       <c r="H34" s="16">
         <f t="shared" si="1"/>
-        <v>22.288</v>
+        <v>14.952000000000002</v>
       </c>
       <c r="I34" s="86" t="s">
-        <v>78</v>
+        <v>145</v>
       </c>
       <c r="J34" s="88" t="s">
         <v>8</v>
@@ -2610,30 +2610,30 @@
     <row r="35" spans="1:10" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="135"/>
       <c r="B35" s="82">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C35" s="83" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D35" s="87" t="s">
         <v>48</v>
       </c>
       <c r="E35" s="87" t="s">
-        <v>81</v>
+        <v>142</v>
       </c>
       <c r="F35" s="18">
-        <v>10.43</v>
+        <v>15.08</v>
       </c>
       <c r="G35" s="4">
         <f t="shared" si="0"/>
-        <v>11.681600000000001</v>
+        <v>16.889600000000002</v>
       </c>
       <c r="H35" s="16">
         <f t="shared" si="1"/>
-        <v>23.363200000000003</v>
+        <v>16.889600000000002</v>
       </c>
       <c r="I35" s="86" t="s">
-        <v>80</v>
+        <v>141</v>
       </c>
       <c r="J35" s="88" t="s">
         <v>8</v>
@@ -2645,13 +2645,13 @@
         <v>1</v>
       </c>
       <c r="C36" s="83" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D36" s="87" t="s">
         <v>48</v>
       </c>
       <c r="E36" s="87" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F36" s="18">
         <v>9.99</v>
@@ -2665,7 +2665,7 @@
         <v>11.188800000000001</v>
       </c>
       <c r="I36" s="86" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J36" s="88" t="s">
         <v>8</v>
@@ -2691,13 +2691,13 @@
         <v>4</v>
       </c>
       <c r="C38" s="83" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D38" s="87" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E38" s="87" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F38" s="18">
         <v>1.6</v>
@@ -2711,7 +2711,7 @@
         <v>7.168000000000001</v>
       </c>
       <c r="I38" s="86" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="J38" s="88" t="s">
         <v>8</v>
@@ -2737,7 +2737,7 @@
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="118" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D40" s="69"/>
       <c r="E40" s="69"/>
@@ -2755,7 +2755,7 @@
         <v>1</v>
       </c>
       <c r="C41" s="118" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D41" s="69"/>
       <c r="E41" s="69"/>
@@ -2781,7 +2781,7 @@
         <v>1</v>
       </c>
       <c r="C42" s="118" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D42" s="69"/>
       <c r="E42" s="69"/>
@@ -3336,10 +3336,10 @@
     <row r="66" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="138"/>
       <c r="B66" s="22" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C66" s="116" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D66" s="37"/>
       <c r="E66" s="35"/>
@@ -3351,10 +3351,10 @@
     <row r="67" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="138"/>
       <c r="B67" s="22" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C67" s="116" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D67" s="37"/>
       <c r="E67" s="35"/>
@@ -3392,7 +3392,7 @@
         <v>1</v>
       </c>
       <c r="C69" s="116" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D69" s="37"/>
       <c r="E69" s="35"/>
@@ -3415,7 +3415,7 @@
         <v>1</v>
       </c>
       <c r="C70" s="116" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D70" s="37"/>
       <c r="E70" s="35"/>
@@ -3438,7 +3438,7 @@
         <v>1</v>
       </c>
       <c r="C71" s="32" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D71" s="37"/>
       <c r="E71" s="35"/>
@@ -3599,7 +3599,7 @@
         <v>1</v>
       </c>
       <c r="C78" s="116" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D78" s="37"/>
       <c r="E78" s="35"/>
@@ -3622,7 +3622,7 @@
         <v>1</v>
       </c>
       <c r="C79" s="116" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D79" s="37"/>
       <c r="E79" s="35"/>
@@ -3645,7 +3645,7 @@
         <v>1</v>
       </c>
       <c r="C80" s="116" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D80" s="37"/>
       <c r="E80" s="35"/>
@@ -3691,7 +3691,7 @@
         <v>1</v>
       </c>
       <c r="C82" s="116" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D82" s="37"/>
       <c r="E82" s="35"/>
@@ -3768,7 +3768,7 @@
     <row r="86" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="138"/>
       <c r="B86" s="143" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C86" s="144"/>
       <c r="D86" s="144"/>
@@ -3784,7 +3784,7 @@
         <v>1</v>
       </c>
       <c r="C87" s="117" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D87" s="54"/>
       <c r="E87" s="54"/>
@@ -3799,7 +3799,7 @@
         <v>1</v>
       </c>
       <c r="C88" s="117" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D88" s="54"/>
       <c r="E88" s="54"/>
@@ -3814,7 +3814,7 @@
         <v>1</v>
       </c>
       <c r="C89" s="116" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D89" s="37"/>
       <c r="E89" s="35"/>
@@ -3829,7 +3829,7 @@
         <v>1</v>
       </c>
       <c r="C90" s="116" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D90" s="37"/>
       <c r="E90" s="35"/>
@@ -3852,7 +3852,7 @@
         <v>1</v>
       </c>
       <c r="C91" s="116" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D91" s="37"/>
       <c r="E91" s="35"/>
@@ -3875,7 +3875,7 @@
         <v>1</v>
       </c>
       <c r="C92" s="116" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D92" s="37"/>
       <c r="E92" s="35"/>
@@ -3898,7 +3898,7 @@
         <v>1</v>
       </c>
       <c r="C93" s="116" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D93" s="37"/>
       <c r="E93" s="35"/>
@@ -3921,7 +3921,7 @@
         <v>1</v>
       </c>
       <c r="C94" s="116" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D94" s="37"/>
       <c r="E94" s="35"/>
@@ -3944,7 +3944,7 @@
         <v>1</v>
       </c>
       <c r="C95" s="116" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D95" s="37"/>
       <c r="E95" s="35"/>
@@ -3967,7 +3967,7 @@
         <v>1</v>
       </c>
       <c r="C96" s="116" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D96" s="37"/>
       <c r="E96" s="35"/>
@@ -3990,7 +3990,7 @@
         <v>1</v>
       </c>
       <c r="C97" s="116" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D97" s="37"/>
       <c r="E97" s="35"/>
@@ -4010,10 +4010,10 @@
     <row r="98" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="138"/>
       <c r="B98" s="22" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C98" s="116" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D98" s="37"/>
       <c r="E98" s="35"/>
@@ -4035,7 +4035,7 @@
         <v>1</v>
       </c>
       <c r="C99" s="116" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D99" s="37"/>
       <c r="E99" s="35"/>
@@ -14831,14 +14831,14 @@
     <hyperlink ref="I21" r:id="rId9" xr:uid="{8DAE0086-1CB4-4A57-9E0C-FD0DC6DDE650}"/>
     <hyperlink ref="I23" r:id="rId10" xr:uid="{0E7F6075-5095-4A84-859E-24E911CCA9A4}"/>
     <hyperlink ref="I33" r:id="rId11" xr:uid="{1B9B6D2F-55F3-4431-803D-BCCE5374B90A}"/>
-    <hyperlink ref="I34" r:id="rId12" xr:uid="{7FC2CA57-66AA-443A-94C2-1F7E1E00ADB2}"/>
-    <hyperlink ref="I35" r:id="rId13" xr:uid="{A4957271-8C33-48E8-A6A4-18B6B9F48E67}"/>
-    <hyperlink ref="I36" r:id="rId14" xr:uid="{B760F12C-A43B-457F-A1FC-943FD6EC5069}"/>
-    <hyperlink ref="I38" r:id="rId15" xr:uid="{AD7CD1B5-E64B-46BD-9C45-7AFE1BA2261E}"/>
-    <hyperlink ref="K25" r:id="rId16" xr:uid="{4896C6AA-E74F-4FD2-94AF-03164218594A}"/>
-    <hyperlink ref="K27" r:id="rId17" xr:uid="{5304B522-7BFB-4401-9BB1-C7AF779A47B6}"/>
-    <hyperlink ref="J27" r:id="rId18" xr:uid="{DA1BC955-C30B-42D2-8DF9-55540D3C26E8}"/>
-    <hyperlink ref="I22" r:id="rId19" xr:uid="{DAE7766D-F4DD-40D5-87EC-5035F7AAC8E9}"/>
+    <hyperlink ref="I36" r:id="rId12" xr:uid="{B760F12C-A43B-457F-A1FC-943FD6EC5069}"/>
+    <hyperlink ref="I38" r:id="rId13" xr:uid="{AD7CD1B5-E64B-46BD-9C45-7AFE1BA2261E}"/>
+    <hyperlink ref="K25" r:id="rId14" xr:uid="{4896C6AA-E74F-4FD2-94AF-03164218594A}"/>
+    <hyperlink ref="K27" r:id="rId15" xr:uid="{5304B522-7BFB-4401-9BB1-C7AF779A47B6}"/>
+    <hyperlink ref="J27" r:id="rId16" xr:uid="{DA1BC955-C30B-42D2-8DF9-55540D3C26E8}"/>
+    <hyperlink ref="I22" r:id="rId17" xr:uid="{DAE7766D-F4DD-40D5-87EC-5035F7AAC8E9}"/>
+    <hyperlink ref="I35" r:id="rId18" xr:uid="{76CB1D51-D078-4B67-8C51-53CF54A0A0AB}"/>
+    <hyperlink ref="I34" r:id="rId19" xr:uid="{A85A737C-E559-492A-97D9-B78CD42A3CD9}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Small update to formatting
</commit_message>
<xml_diff>
--- a/TurbofanDriver - V3 Bill of Materials.xlsx
+++ b/TurbofanDriver - V3 Bill of Materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/844add23945bcd8f/Documents/3D Printer Shit/1___3D_Printable_Jet_Engine_Upgrade/V3 Upgrades/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1081" documentId="13_ncr:1_{2F400004-E652-4E60-AF98-6B4D8D866B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4C6C95B-F6FF-4241-84FD-A1367AAD4DD6}"/>
+  <xr:revisionPtr revIDLastSave="1092" documentId="13_ncr:1_{2F400004-E652-4E60-AF98-6B4D8D866B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5DB7829-6BEE-4F9F-A426-F811C7E92036}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -631,7 +631,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -863,24 +863,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -889,19 +871,6 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1059,12 +1028,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1137,12 +1128,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1205,9 +1190,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1215,7 +1197,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1224,35 +1206,35 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1261,49 +1243,10 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1321,19 +1264,64 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1558,17 +1546,17 @@
   </sheetPr>
   <dimension ref="A1:L856"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.140625" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" customWidth="1"/>
     <col min="3" max="3" width="102.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" style="21" bestFit="1" customWidth="1"/>
@@ -1578,36 +1566,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="82" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
     </row>
     <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
     </row>
     <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="77"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
+      <c r="B3" s="83"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="83"/>
     </row>
     <row r="4" spans="1:11" s="21" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -1616,14 +1604,14 @@
       <c r="B4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="66"/>
-      <c r="G4" s="66" t="s">
+      <c r="C4" s="63"/>
+      <c r="G4" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="H4" s="69" t="s">
+      <c r="H4" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="68"/>
+      <c r="I4" s="65"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="84" t="s">
@@ -1638,15 +1626,15 @@
       <c r="D5" s="20"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="74">
+      <c r="G5" s="80">
         <v>225</v>
       </c>
-      <c r="H5" s="74">
+      <c r="H5" s="80">
         <f xml:space="preserve"> H7+H9</f>
         <v>349.18986666666672</v>
       </c>
-      <c r="I5" s="67"/>
-      <c r="J5" s="47" t="s">
+      <c r="I5" s="64"/>
+      <c r="J5" s="45" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1658,9 +1646,9 @@
       <c r="D6" s="20"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="75"/>
-      <c r="I6" s="64"/>
+      <c r="G6" s="81"/>
+      <c r="H6" s="81"/>
+      <c r="I6" s="61"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="85"/>
@@ -1673,14 +1661,14 @@
       <c r="D7" s="10"/>
       <c r="E7" s="23"/>
       <c r="F7" s="23"/>
-      <c r="G7" s="61">
+      <c r="G7" s="58">
         <v>0</v>
       </c>
-      <c r="H7" s="65">
+      <c r="H7" s="62">
         <f>SUM(H14:H29)</f>
         <v>249.59573333333336</v>
       </c>
-      <c r="I7" s="63"/>
+      <c r="I7" s="60"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="85"/>
@@ -1691,13 +1679,13 @@
       <c r="D8" s="10"/>
       <c r="E8" s="23"/>
       <c r="F8" s="23"/>
-      <c r="G8" s="61">
+      <c r="G8" s="58">
         <v>160</v>
       </c>
-      <c r="H8" s="61">
+      <c r="H8" s="58">
         <v>0</v>
       </c>
-      <c r="I8" s="63"/>
+      <c r="I8" s="60"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="85"/>
@@ -1710,14 +1698,14 @@
       <c r="D9" s="10"/>
       <c r="E9" s="23"/>
       <c r="F9" s="23"/>
-      <c r="G9" s="61">
+      <c r="G9" s="58">
         <v>0</v>
       </c>
-      <c r="H9" s="62">
+      <c r="H9" s="59">
         <f>SUM(H32:H38)</f>
         <v>99.594133333333346</v>
       </c>
-      <c r="I9" s="63"/>
+      <c r="I9" s="60"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="85"/>
@@ -1728,80 +1716,80 @@
       <c r="D10" s="10"/>
       <c r="E10" s="23"/>
       <c r="F10" s="23"/>
-      <c r="G10" s="61">
+      <c r="G10" s="58">
         <v>75</v>
       </c>
-      <c r="H10" s="61">
+      <c r="H10" s="58">
         <v>0</v>
       </c>
-      <c r="I10" s="63"/>
-    </row>
-    <row r="11" spans="1:11" s="33" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="60"/>
+    </row>
+    <row r="11" spans="1:11" s="31" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="86"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="32"/>
-    </row>
-    <row r="12" spans="1:11" s="44" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="78" t="s">
+      <c r="B11" s="27"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="30"/>
+    </row>
+    <row r="12" spans="1:11" s="42" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="84" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="70"/>
-      <c r="D12" s="66" t="s">
+      <c r="B12" s="94"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="66" t="s">
+      <c r="E12" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="71" t="s">
+      <c r="F12" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="G12" s="71" t="s">
+      <c r="G12" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="H12" s="66" t="s">
+      <c r="H12" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="66" t="s">
+      <c r="I12" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="J12" s="66" t="s">
+      <c r="J12" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="K12" s="66" t="s">
+      <c r="K12" s="63" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="44" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="79"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
+    <row r="13" spans="1:11" s="42" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="85"/>
+      <c r="B13" s="94"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
       <c r="F13" s="12"/>
       <c r="G13" s="4"/>
       <c r="H13" s="12"/>
-      <c r="I13" s="43"/>
+      <c r="I13" s="41"/>
       <c r="J13"/>
     </row>
-    <row r="14" spans="1:11" s="44" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="79"/>
-      <c r="B14" s="41">
+    <row r="14" spans="1:11" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="85"/>
+      <c r="B14" s="94">
         <v>1</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="46" t="s">
+      <c r="D14" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="46" t="s">
+      <c r="E14" s="44" t="s">
         <v>17</v>
       </c>
       <c r="F14" s="14">
@@ -1815,25 +1803,25 @@
         <f>B14*G14</f>
         <v>36.948800000000006</v>
       </c>
-      <c r="I14" s="45" t="s">
+      <c r="I14" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="J14" s="47" t="s">
+      <c r="J14" s="45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="44" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="79"/>
-      <c r="B15" s="41">
+    <row r="15" spans="1:11" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="85"/>
+      <c r="B15" s="94">
         <v>1</v>
       </c>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="46" t="s">
+      <c r="D15" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="46" t="s">
+      <c r="E15" s="44" t="s">
         <v>23</v>
       </c>
       <c r="F15" s="14">
@@ -1847,25 +1835,25 @@
         <f t="shared" ref="H15:H38" si="1">B15*G15</f>
         <v>12.040000000000001</v>
       </c>
-      <c r="I15" s="48" t="s">
+      <c r="I15" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="J15" s="47" t="s">
+      <c r="J15" s="45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="44" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="79"/>
-      <c r="B16" s="41">
+    <row r="16" spans="1:11" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="85"/>
+      <c r="B16" s="94">
         <v>1</v>
       </c>
-      <c r="C16" s="42" t="s">
+      <c r="C16" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="46" t="s">
+      <c r="D16" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="46" t="s">
+      <c r="E16" s="44" t="s">
         <v>31</v>
       </c>
       <c r="F16" s="14">
@@ -1879,25 +1867,25 @@
         <f t="shared" si="1"/>
         <v>13.305600000000002</v>
       </c>
-      <c r="I16" s="45" t="s">
+      <c r="I16" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="J16" s="47" t="s">
+      <c r="J16" s="45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="44" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="79"/>
-      <c r="B17" s="41">
+    <row r="17" spans="1:12" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="85"/>
+      <c r="B17" s="94">
         <v>1</v>
       </c>
-      <c r="C17" s="42" t="s">
+      <c r="C17" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="D17" s="46" t="s">
+      <c r="D17" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="46" t="s">
+      <c r="E17" s="44" t="s">
         <v>54</v>
       </c>
       <c r="F17" s="14">
@@ -1911,25 +1899,25 @@
         <f t="shared" si="1"/>
         <v>15.668800000000001</v>
       </c>
-      <c r="I17" s="45" t="s">
+      <c r="I17" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="J17" s="47" t="s">
+      <c r="J17" s="45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="44" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="79"/>
-      <c r="B18" s="41">
+    <row r="18" spans="1:12" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="85"/>
+      <c r="B18" s="94">
         <v>1</v>
       </c>
-      <c r="C18" s="42" t="s">
+      <c r="C18" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="46" t="s">
+      <c r="D18" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="46" t="s">
+      <c r="E18" s="44" t="s">
         <v>33</v>
       </c>
       <c r="F18" s="14">
@@ -1943,25 +1931,25 @@
         <f t="shared" si="1"/>
         <v>33.745600000000003</v>
       </c>
-      <c r="I18" s="45" t="s">
+      <c r="I18" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="J18" s="47" t="s">
+      <c r="J18" s="45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="44" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="79"/>
-      <c r="B19" s="41">
+    <row r="19" spans="1:12" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="85"/>
+      <c r="B19" s="94">
         <v>1</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="C19" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="46" t="s">
+      <c r="D19" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="46" t="s">
+      <c r="E19" s="44" t="s">
         <v>20</v>
       </c>
       <c r="F19" s="14">
@@ -1975,25 +1963,25 @@
         <f t="shared" si="1"/>
         <v>12.801600000000001</v>
       </c>
-      <c r="I19" s="45" t="s">
+      <c r="I19" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J19" s="47" t="s">
+      <c r="J19" s="45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="44" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="79"/>
-      <c r="B20" s="41">
+    <row r="20" spans="1:12" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="85"/>
+      <c r="B20" s="94">
         <v>1</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="46" t="s">
+      <c r="D20" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="46" t="s">
+      <c r="E20" s="44" t="s">
         <v>37</v>
       </c>
       <c r="F20" s="14">
@@ -2007,25 +1995,25 @@
         <f t="shared" si="1"/>
         <v>17.908800000000003</v>
       </c>
-      <c r="I20" s="45" t="s">
+      <c r="I20" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="47" t="s">
+      <c r="J20" s="45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="44" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="79"/>
-      <c r="B21" s="41">
+    <row r="21" spans="1:12" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="85"/>
+      <c r="B21" s="94">
         <v>1</v>
       </c>
-      <c r="C21" s="42" t="s">
+      <c r="C21" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="46" t="s">
+      <c r="D21" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="46" t="s">
+      <c r="E21" s="44" t="s">
         <v>40</v>
       </c>
       <c r="F21" s="14">
@@ -2039,25 +2027,25 @@
         <f t="shared" si="1"/>
         <v>17.908800000000003</v>
       </c>
-      <c r="I21" s="45" t="s">
+      <c r="I21" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="J21" s="47" t="s">
+      <c r="J21" s="45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="44" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="79"/>
-      <c r="B22" s="41">
+    <row r="22" spans="1:12" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="85"/>
+      <c r="B22" s="94">
         <v>1</v>
       </c>
-      <c r="C22" s="42" t="s">
+      <c r="C22" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="D22" s="46" t="s">
+      <c r="D22" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="46" t="s">
+      <c r="E22" s="44" t="s">
         <v>91</v>
       </c>
       <c r="F22" s="14">
@@ -2071,25 +2059,25 @@
         <f t="shared" si="1"/>
         <v>20.148800000000001</v>
       </c>
-      <c r="I22" s="45" t="s">
+      <c r="I22" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="J22" s="47" t="s">
+      <c r="J22" s="45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="44" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="79"/>
-      <c r="B23" s="41">
+    <row r="23" spans="1:12" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="85"/>
+      <c r="B23" s="94">
         <v>1</v>
       </c>
-      <c r="C23" s="42" t="s">
+      <c r="C23" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="46" t="s">
+      <c r="D23" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="46" t="s">
+      <c r="E23" s="44" t="s">
         <v>42</v>
       </c>
       <c r="F23" s="14">
@@ -2103,37 +2091,37 @@
         <f t="shared" si="1"/>
         <v>26.8688</v>
       </c>
-      <c r="I23" s="45" t="s">
+      <c r="I23" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="J23" s="47" t="s">
+      <c r="J23" s="45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="44" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="79"/>
-      <c r="B24" s="41"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="46"/>
-      <c r="E24" s="46"/>
+    <row r="24" spans="1:12" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="85"/>
+      <c r="B24" s="94"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
       <c r="F24" s="14"/>
       <c r="G24" s="4"/>
       <c r="H24" s="12"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="49"/>
-    </row>
-    <row r="25" spans="1:12" s="44" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="79"/>
-      <c r="B25" s="41">
+      <c r="I24" s="43"/>
+      <c r="J24" s="47"/>
+    </row>
+    <row r="25" spans="1:12" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="85"/>
+      <c r="B25" s="94">
         <v>1</v>
       </c>
-      <c r="C25" s="42" t="s">
+      <c r="C25" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="46" t="s">
+      <c r="D25" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="46" t="s">
+      <c r="E25" s="44" t="s">
         <v>25</v>
       </c>
       <c r="F25" s="14">
@@ -2148,43 +2136,43 @@
         <f>B25*G25</f>
         <v>14.918400000000002</v>
       </c>
-      <c r="I25" s="45" t="s">
+      <c r="I25" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="J25" s="47" t="s">
+      <c r="J25" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="K25" s="48" t="s">
+      <c r="K25" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="L25" s="47" t="s">
+      <c r="L25" s="45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="44" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="79"/>
-      <c r="B26" s="41"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
+    <row r="26" spans="1:12" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="85"/>
+      <c r="B26" s="94"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
       <c r="F26" s="14"/>
       <c r="G26" s="4"/>
       <c r="H26" s="12"/>
-      <c r="I26" s="45"/>
-      <c r="J26" s="49"/>
-    </row>
-    <row r="27" spans="1:12" s="44" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="79"/>
-      <c r="B27" s="41">
+      <c r="I26" s="43"/>
+      <c r="J26" s="47"/>
+    </row>
+    <row r="27" spans="1:12" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="85"/>
+      <c r="B27" s="94">
         <v>1</v>
       </c>
-      <c r="C27" s="42" t="s">
+      <c r="C27" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="46" t="s">
+      <c r="D27" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="E27" s="46" t="s">
+      <c r="E27" s="44" t="s">
         <v>29</v>
       </c>
       <c r="F27" s="14">
@@ -2199,43 +2187,43 @@
         <f>B27*G27</f>
         <v>21.877333333333336</v>
       </c>
-      <c r="I27" s="45" t="s">
+      <c r="I27" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="J27" s="45" t="s">
+      <c r="J27" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="K27" s="48" t="s">
+      <c r="K27" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="L27" s="47" t="s">
+      <c r="L27" s="45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="56" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="79"/>
-      <c r="B28" s="41"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="46"/>
-      <c r="E28" s="46"/>
+    <row r="28" spans="1:12" s="53" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="85"/>
+      <c r="B28" s="94"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
       <c r="F28" s="14"/>
       <c r="G28" s="4"/>
       <c r="H28" s="12"/>
-      <c r="I28" s="55"/>
-      <c r="J28" s="47"/>
-    </row>
-    <row r="29" spans="1:12" s="56" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="79"/>
-      <c r="B29" s="54">
+      <c r="I28" s="52"/>
+      <c r="J28" s="45"/>
+    </row>
+    <row r="29" spans="1:12" s="53" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="85"/>
+      <c r="B29" s="97">
         <v>1</v>
       </c>
-      <c r="C29" s="42" t="s">
+      <c r="C29" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="D29" s="46" t="s">
+      <c r="D29" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="E29" s="59" t="s">
+      <c r="E29" s="56" t="s">
         <v>8</v>
       </c>
       <c r="F29" s="14">
@@ -2245,57 +2233,57 @@
         <f>F29*1.12</f>
         <v>5.4544000000000006</v>
       </c>
-      <c r="H29" s="58">
+      <c r="H29" s="55">
         <f>B29*G29</f>
         <v>5.4544000000000006</v>
       </c>
-      <c r="I29" s="60" t="s">
+      <c r="I29" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="J29" s="47"/>
-    </row>
-    <row r="30" spans="1:12" s="53" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="80"/>
-      <c r="B30" s="35"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="57"/>
+      <c r="J29" s="45"/>
+    </row>
+    <row r="30" spans="1:12" s="51" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="86"/>
+      <c r="B30" s="96"/>
+      <c r="C30" s="48"/>
+      <c r="D30" s="54"/>
+      <c r="E30" s="54"/>
       <c r="F30" s="13"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="51"/>
-      <c r="J30" s="52" t="s">
+      <c r="G30" s="28"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="49"/>
+      <c r="J30" s="50" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="44" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="81" t="s">
+    <row r="31" spans="1:12" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="41"/>
-      <c r="C31" s="42"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="41"/>
+      <c r="B31" s="94"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
       <c r="F31" s="12"/>
       <c r="G31" s="4"/>
       <c r="H31" s="12"/>
-      <c r="I31" s="43"/>
-      <c r="J31" s="47" t="s">
+      <c r="I31" s="41"/>
+      <c r="J31" s="45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="44" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="82"/>
-      <c r="B32" s="41">
+    <row r="32" spans="1:12" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="85"/>
+      <c r="B32" s="94">
         <v>1</v>
       </c>
-      <c r="C32" s="42" t="s">
+      <c r="C32" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="D32" s="46" t="s">
+      <c r="D32" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="E32" s="46" t="s">
+      <c r="E32" s="44" t="s">
         <v>80</v>
       </c>
       <c r="F32" s="14">
@@ -2309,25 +2297,25 @@
         <f t="shared" ref="H32" si="2">B32*G32</f>
         <v>17.908800000000003</v>
       </c>
-      <c r="I32" s="45" t="s">
+      <c r="I32" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="J32" s="47" t="s">
+      <c r="J32" s="45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="44" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="82"/>
-      <c r="B33" s="46" t="s">
+    <row r="33" spans="1:10" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="85"/>
+      <c r="B33" s="95" t="s">
         <v>87</v>
       </c>
-      <c r="C33" s="42" t="s">
+      <c r="C33" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="D33" s="46" t="s">
+      <c r="D33" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="E33" s="46" t="s">
+      <c r="E33" s="44" t="s">
         <v>84</v>
       </c>
       <c r="F33" s="14">
@@ -2341,25 +2329,25 @@
         <f>2*G33</f>
         <v>29.097600000000003</v>
       </c>
-      <c r="I33" s="45" t="s">
+      <c r="I33" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="J33" s="47" t="s">
+      <c r="J33" s="45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="44" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="82"/>
-      <c r="B34" s="41">
+    <row r="34" spans="1:10" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="85"/>
+      <c r="B34" s="94">
         <v>1</v>
       </c>
-      <c r="C34" s="42" t="s">
+      <c r="C34" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="D34" s="46" t="s">
+      <c r="D34" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="E34" s="46" t="s">
+      <c r="E34" s="44" t="s">
         <v>97</v>
       </c>
       <c r="F34" s="14">
@@ -2373,25 +2361,25 @@
         <f t="shared" si="1"/>
         <v>14.952000000000002</v>
       </c>
-      <c r="I34" s="45" t="s">
+      <c r="I34" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="J34" s="47" t="s">
+      <c r="J34" s="45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="44" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="82"/>
-      <c r="B35" s="41">
+    <row r="35" spans="1:10" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="85"/>
+      <c r="B35" s="94">
         <v>1</v>
       </c>
-      <c r="C35" s="42" t="s">
+      <c r="C35" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="D35" s="46" t="s">
+      <c r="D35" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="E35" s="46" t="s">
+      <c r="E35" s="44" t="s">
         <v>93</v>
       </c>
       <c r="F35" s="14">
@@ -2405,25 +2393,25 @@
         <f t="shared" si="1"/>
         <v>16.889600000000002</v>
       </c>
-      <c r="I35" s="45" t="s">
+      <c r="I35" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="J35" s="47" t="s">
+      <c r="J35" s="45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="44" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="82"/>
-      <c r="B36" s="41">
+    <row r="36" spans="1:10" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="85"/>
+      <c r="B36" s="94">
         <v>1</v>
       </c>
-      <c r="C36" s="42" t="s">
+      <c r="C36" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="D36" s="46" t="s">
+      <c r="D36" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="E36" s="46" t="s">
+      <c r="E36" s="44" t="s">
         <v>47</v>
       </c>
       <c r="F36" s="14">
@@ -2437,39 +2425,39 @@
         <f t="shared" si="1"/>
         <v>11.188800000000001</v>
       </c>
-      <c r="I36" s="45" t="s">
+      <c r="I36" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="J36" s="47" t="s">
+      <c r="J36" s="45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="44" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="82"/>
-      <c r="B37" s="41"/>
-      <c r="C37" s="42"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="41"/>
+    <row r="37" spans="1:10" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="85"/>
+      <c r="B37" s="94"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="39"/>
       <c r="F37" s="14"/>
       <c r="G37" s="4"/>
       <c r="H37" s="12"/>
-      <c r="I37" s="43"/>
-      <c r="J37" s="47" t="s">
+      <c r="I37" s="41"/>
+      <c r="J37" s="45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="44" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="82"/>
-      <c r="B38" s="41">
+    <row r="38" spans="1:10" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="85"/>
+      <c r="B38" s="94">
         <v>4</v>
       </c>
-      <c r="C38" s="42" t="s">
+      <c r="C38" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="D38" s="46" t="s">
+      <c r="D38" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="E38" s="46" t="s">
+      <c r="E38" s="44" t="s">
         <v>50</v>
       </c>
       <c r="F38" s="14">
@@ -2484,63 +2472,63 @@
         <f t="shared" si="1"/>
         <v>9.5573333333333341</v>
       </c>
-      <c r="I38" s="45" t="s">
+      <c r="I38" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="J38" s="47" t="s">
+      <c r="J38" s="45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="40" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="83"/>
-      <c r="B39" s="35"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="35"/>
-      <c r="E39" s="35"/>
-      <c r="F39" s="37"/>
-      <c r="G39" s="38"/>
-      <c r="H39" s="37"/>
-      <c r="I39" s="39"/>
-      <c r="J39" s="47" t="s">
+    <row r="39" spans="1:10" s="38" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="86"/>
+      <c r="B39" s="96"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="35"/>
+      <c r="G39" s="36"/>
+      <c r="H39" s="35"/>
+      <c r="I39" s="37"/>
+      <c r="J39" s="45" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="26" t="s">
+      <c r="A40" s="90" t="s">
         <v>11</v>
       </c>
       <c r="B40" s="3"/>
-      <c r="C40" s="73" t="s">
+      <c r="C40" s="70" t="s">
         <v>73</v>
       </c>
-      <c r="D40" s="28"/>
-      <c r="E40" s="28"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
       <c r="F40" s="12"/>
       <c r="G40" s="4"/>
       <c r="H40" s="12"/>
       <c r="I40" s="17"/>
-      <c r="J40" s="47" t="s">
+      <c r="J40" s="45" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="27"/>
-      <c r="B41" s="97"/>
-      <c r="C41" s="87"/>
-      <c r="D41" s="98"/>
-      <c r="E41" s="98"/>
+      <c r="A41" s="91"/>
+      <c r="B41" s="78"/>
+      <c r="C41" s="71"/>
+      <c r="D41" s="79"/>
+      <c r="E41" s="79"/>
       <c r="F41" s="12"/>
       <c r="G41" s="4"/>
       <c r="H41" s="12"/>
       <c r="I41" s="22"/>
-      <c r="J41" s="47"/>
+      <c r="J41" s="45"/>
     </row>
     <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="27"/>
+      <c r="A42" s="91"/>
       <c r="B42" s="16">
         <v>1</v>
       </c>
-      <c r="C42" s="72" t="s">
+      <c r="C42" s="69" t="s">
         <v>102</v>
       </c>
       <c r="D42" s="25"/>
@@ -2551,944 +2539,944 @@
       <c r="I42" s="22"/>
     </row>
     <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="27"/>
-      <c r="B43" s="88">
+      <c r="A43" s="91"/>
+      <c r="B43" s="72">
         <v>1</v>
       </c>
-      <c r="C43" s="89" t="s">
+      <c r="C43" s="73" t="s">
         <v>103</v>
       </c>
-      <c r="D43" s="91"/>
-      <c r="E43" s="92"/>
-      <c r="F43" s="90"/>
+      <c r="D43" s="75"/>
+      <c r="E43" s="76"/>
+      <c r="F43" s="74"/>
       <c r="G43" s="4"/>
       <c r="H43" s="12"/>
       <c r="I43" s="22"/>
     </row>
     <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="27"/>
-      <c r="B44" s="88">
+      <c r="A44" s="91"/>
+      <c r="B44" s="72">
         <v>1</v>
       </c>
-      <c r="C44" s="89" t="s">
+      <c r="C44" s="73" t="s">
         <v>104</v>
       </c>
-      <c r="D44" s="91"/>
-      <c r="E44" s="92"/>
-      <c r="F44" s="90"/>
+      <c r="D44" s="75"/>
+      <c r="E44" s="76"/>
+      <c r="F44" s="74"/>
       <c r="G44" s="4"/>
       <c r="H44" s="12"/>
       <c r="I44" s="22"/>
     </row>
     <row r="45" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="27"/>
-      <c r="B45" s="88">
+      <c r="A45" s="91"/>
+      <c r="B45" s="72">
         <v>1</v>
       </c>
-      <c r="C45" s="93" t="s">
+      <c r="C45" s="77" t="s">
         <v>105</v>
       </c>
-      <c r="D45" s="91"/>
-      <c r="E45" s="92"/>
-      <c r="F45" s="90"/>
+      <c r="D45" s="75"/>
+      <c r="E45" s="76"/>
+      <c r="F45" s="74"/>
       <c r="G45" s="4"/>
       <c r="H45" s="12"/>
       <c r="I45" s="22"/>
     </row>
     <row r="46" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="27"/>
-      <c r="B46" s="88">
+      <c r="A46" s="91"/>
+      <c r="B46" s="72">
         <v>1</v>
       </c>
-      <c r="C46" s="89" t="s">
+      <c r="C46" s="73" t="s">
         <v>106</v>
       </c>
-      <c r="D46" s="91"/>
-      <c r="E46" s="92"/>
-      <c r="F46" s="90"/>
+      <c r="D46" s="75"/>
+      <c r="E46" s="76"/>
+      <c r="F46" s="74"/>
       <c r="G46" s="4"/>
       <c r="H46" s="12"/>
       <c r="I46" s="22"/>
     </row>
     <row r="47" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="27"/>
-      <c r="B47" s="88">
+      <c r="A47" s="91"/>
+      <c r="B47" s="72">
         <v>1</v>
       </c>
-      <c r="C47" s="93" t="s">
+      <c r="C47" s="77" t="s">
         <v>107</v>
       </c>
-      <c r="D47" s="91"/>
-      <c r="E47" s="92"/>
-      <c r="F47" s="90"/>
+      <c r="D47" s="75"/>
+      <c r="E47" s="76"/>
+      <c r="F47" s="74"/>
       <c r="G47" s="4"/>
       <c r="H47" s="12"/>
       <c r="I47" s="22"/>
     </row>
     <row r="48" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="27"/>
-      <c r="B48" s="88">
+      <c r="A48" s="91"/>
+      <c r="B48" s="72">
         <v>1</v>
       </c>
-      <c r="C48" s="93" t="s">
+      <c r="C48" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="D48" s="91"/>
-      <c r="E48" s="92"/>
-      <c r="F48" s="90"/>
+      <c r="D48" s="75"/>
+      <c r="E48" s="76"/>
+      <c r="F48" s="74"/>
       <c r="G48" s="4"/>
       <c r="H48" s="12"/>
       <c r="I48" s="22"/>
     </row>
     <row r="49" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="27"/>
-      <c r="B49" s="88">
+      <c r="A49" s="91"/>
+      <c r="B49" s="72">
         <v>1</v>
       </c>
-      <c r="C49" s="89" t="s">
+      <c r="C49" s="73" t="s">
         <v>109</v>
       </c>
-      <c r="D49" s="91"/>
-      <c r="E49" s="92"/>
-      <c r="F49" s="90"/>
+      <c r="D49" s="75"/>
+      <c r="E49" s="76"/>
+      <c r="F49" s="74"/>
       <c r="G49" s="4"/>
       <c r="H49" s="12"/>
       <c r="I49" s="22"/>
     </row>
     <row r="50" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="27"/>
-      <c r="B50" s="88">
+      <c r="A50" s="91"/>
+      <c r="B50" s="72">
         <v>1</v>
       </c>
-      <c r="C50" s="89" t="s">
+      <c r="C50" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="D50" s="91"/>
-      <c r="E50" s="92"/>
-      <c r="F50" s="90"/>
+      <c r="D50" s="75"/>
+      <c r="E50" s="76"/>
+      <c r="F50" s="74"/>
       <c r="G50" s="4"/>
       <c r="H50" s="12"/>
       <c r="I50" s="22"/>
     </row>
     <row r="51" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="27"/>
-      <c r="B51" s="88">
+      <c r="A51" s="91"/>
+      <c r="B51" s="72">
         <v>1</v>
       </c>
-      <c r="C51" s="93" t="s">
+      <c r="C51" s="77" t="s">
         <v>111</v>
       </c>
-      <c r="D51" s="91"/>
-      <c r="E51" s="92"/>
-      <c r="F51" s="90"/>
+      <c r="D51" s="75"/>
+      <c r="E51" s="76"/>
+      <c r="F51" s="74"/>
       <c r="G51" s="4"/>
       <c r="H51" s="12"/>
       <c r="I51" s="22"/>
     </row>
     <row r="52" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="27"/>
-      <c r="B52" s="88">
+      <c r="A52" s="91"/>
+      <c r="B52" s="72">
         <v>1</v>
       </c>
-      <c r="C52" s="89" t="s">
+      <c r="C52" s="73" t="s">
         <v>112</v>
       </c>
-      <c r="D52" s="91"/>
-      <c r="E52" s="92"/>
-      <c r="F52" s="90"/>
+      <c r="D52" s="75"/>
+      <c r="E52" s="76"/>
+      <c r="F52" s="74"/>
       <c r="G52" s="4"/>
       <c r="H52" s="12"/>
       <c r="I52" s="22"/>
     </row>
     <row r="53" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="27"/>
-      <c r="B53" s="88">
+      <c r="A53" s="91"/>
+      <c r="B53" s="72">
         <v>1</v>
       </c>
-      <c r="C53" s="89" t="s">
+      <c r="C53" s="73" t="s">
         <v>113</v>
       </c>
-      <c r="D53" s="91"/>
-      <c r="E53" s="92"/>
-      <c r="F53" s="90"/>
+      <c r="D53" s="75"/>
+      <c r="E53" s="76"/>
+      <c r="F53" s="74"/>
       <c r="G53" s="4"/>
       <c r="H53" s="12"/>
       <c r="I53" s="22"/>
     </row>
     <row r="54" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="27"/>
-      <c r="B54" s="88">
+      <c r="A54" s="91"/>
+      <c r="B54" s="72">
         <v>1</v>
       </c>
-      <c r="C54" s="89" t="s">
+      <c r="C54" s="73" t="s">
         <v>114</v>
       </c>
-      <c r="D54" s="91"/>
-      <c r="E54" s="92"/>
-      <c r="F54" s="90"/>
+      <c r="D54" s="75"/>
+      <c r="E54" s="76"/>
+      <c r="F54" s="74"/>
       <c r="G54" s="4"/>
       <c r="H54" s="12"/>
       <c r="I54" s="22"/>
     </row>
     <row r="55" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="27"/>
-      <c r="B55" s="88">
+      <c r="A55" s="91"/>
+      <c r="B55" s="72">
         <v>1</v>
       </c>
-      <c r="C55" s="89" t="s">
+      <c r="C55" s="73" t="s">
         <v>115</v>
       </c>
-      <c r="D55" s="91"/>
-      <c r="E55" s="92"/>
-      <c r="F55" s="90"/>
+      <c r="D55" s="75"/>
+      <c r="E55" s="76"/>
+      <c r="F55" s="74"/>
       <c r="G55" s="4"/>
       <c r="H55" s="12"/>
       <c r="I55" s="22"/>
     </row>
     <row r="56" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="27"/>
-      <c r="B56" s="88">
+      <c r="A56" s="91"/>
+      <c r="B56" s="72">
         <v>1</v>
       </c>
-      <c r="C56" s="89" t="s">
+      <c r="C56" s="73" t="s">
         <v>116</v>
       </c>
-      <c r="D56" s="91"/>
-      <c r="E56" s="92"/>
-      <c r="F56" s="90"/>
+      <c r="D56" s="75"/>
+      <c r="E56" s="76"/>
+      <c r="F56" s="74"/>
       <c r="G56" s="4"/>
       <c r="H56" s="12"/>
       <c r="I56" s="22"/>
     </row>
     <row r="57" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="27"/>
-      <c r="B57" s="88">
+      <c r="A57" s="91"/>
+      <c r="B57" s="72">
         <v>1</v>
       </c>
-      <c r="C57" s="89" t="s">
+      <c r="C57" s="73" t="s">
         <v>117</v>
       </c>
-      <c r="D57" s="91"/>
-      <c r="E57" s="92"/>
-      <c r="F57" s="90"/>
+      <c r="D57" s="75"/>
+      <c r="E57" s="76"/>
+      <c r="F57" s="74"/>
       <c r="G57" s="4"/>
       <c r="H57" s="12"/>
       <c r="I57" s="22"/>
     </row>
     <row r="58" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="27"/>
-      <c r="B58" s="88">
+      <c r="A58" s="91"/>
+      <c r="B58" s="72">
         <v>1</v>
       </c>
-      <c r="C58" s="89" t="s">
+      <c r="C58" s="73" t="s">
         <v>118</v>
       </c>
-      <c r="D58" s="91"/>
-      <c r="E58" s="92"/>
-      <c r="F58" s="90"/>
+      <c r="D58" s="75"/>
+      <c r="E58" s="76"/>
+      <c r="F58" s="74"/>
       <c r="G58" s="4"/>
       <c r="H58" s="12"/>
       <c r="I58" s="22"/>
     </row>
     <row r="59" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="27"/>
-      <c r="B59" s="88">
+      <c r="A59" s="91"/>
+      <c r="B59" s="72">
         <v>1</v>
       </c>
-      <c r="C59" s="89" t="s">
+      <c r="C59" s="73" t="s">
         <v>119</v>
       </c>
-      <c r="D59" s="91"/>
-      <c r="E59" s="92"/>
-      <c r="F59" s="90"/>
+      <c r="D59" s="75"/>
+      <c r="E59" s="76"/>
+      <c r="F59" s="74"/>
       <c r="G59" s="4"/>
       <c r="H59" s="12"/>
       <c r="I59" s="22"/>
     </row>
     <row r="60" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="27"/>
-      <c r="B60" s="88">
+      <c r="A60" s="91"/>
+      <c r="B60" s="72">
         <v>1</v>
       </c>
-      <c r="C60" s="89" t="s">
+      <c r="C60" s="73" t="s">
         <v>120</v>
       </c>
-      <c r="D60" s="91"/>
-      <c r="E60" s="92"/>
-      <c r="F60" s="90"/>
+      <c r="D60" s="75"/>
+      <c r="E60" s="76"/>
+      <c r="F60" s="74"/>
       <c r="G60" s="4"/>
       <c r="H60" s="12"/>
       <c r="I60" s="22"/>
     </row>
     <row r="61" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="27"/>
-      <c r="B61" s="88">
+      <c r="A61" s="91"/>
+      <c r="B61" s="72">
         <v>1</v>
       </c>
-      <c r="C61" s="89" t="s">
+      <c r="C61" s="73" t="s">
         <v>121</v>
       </c>
-      <c r="D61" s="91"/>
-      <c r="E61" s="92"/>
-      <c r="F61" s="90"/>
+      <c r="D61" s="75"/>
+      <c r="E61" s="76"/>
+      <c r="F61" s="74"/>
       <c r="G61" s="4"/>
       <c r="H61" s="12"/>
       <c r="I61" s="22"/>
     </row>
     <row r="62" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="27"/>
-      <c r="B62" s="88">
+      <c r="A62" s="91"/>
+      <c r="B62" s="72">
         <v>1</v>
       </c>
-      <c r="C62" s="89" t="s">
+      <c r="C62" s="73" t="s">
         <v>122</v>
       </c>
-      <c r="D62" s="91"/>
-      <c r="E62" s="92"/>
-      <c r="F62" s="90"/>
+      <c r="D62" s="75"/>
+      <c r="E62" s="76"/>
+      <c r="F62" s="74"/>
       <c r="G62" s="4"/>
       <c r="H62" s="12"/>
       <c r="I62" s="22"/>
     </row>
     <row r="63" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="27"/>
-      <c r="B63" s="88">
+      <c r="A63" s="91"/>
+      <c r="B63" s="72">
         <v>1</v>
       </c>
-      <c r="C63" s="89" t="s">
+      <c r="C63" s="73" t="s">
         <v>123</v>
       </c>
-      <c r="D63" s="91"/>
-      <c r="E63" s="92"/>
-      <c r="F63" s="90"/>
+      <c r="D63" s="75"/>
+      <c r="E63" s="76"/>
+      <c r="F63" s="74"/>
       <c r="G63" s="4"/>
       <c r="H63" s="12"/>
       <c r="I63" s="22"/>
     </row>
     <row r="64" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="27"/>
-      <c r="B64" s="88">
+      <c r="A64" s="91"/>
+      <c r="B64" s="72">
         <v>1</v>
       </c>
-      <c r="C64" s="89" t="s">
+      <c r="C64" s="73" t="s">
         <v>124</v>
       </c>
-      <c r="D64" s="91"/>
-      <c r="E64" s="92"/>
-      <c r="F64" s="90"/>
+      <c r="D64" s="75"/>
+      <c r="E64" s="76"/>
+      <c r="F64" s="74"/>
       <c r="G64" s="4"/>
       <c r="H64" s="12"/>
       <c r="I64" s="22"/>
     </row>
     <row r="65" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="27"/>
-      <c r="B65" s="88">
+      <c r="A65" s="91"/>
+      <c r="B65" s="72">
         <v>1</v>
       </c>
-      <c r="C65" s="89" t="s">
+      <c r="C65" s="73" t="s">
         <v>125</v>
       </c>
-      <c r="D65" s="91"/>
-      <c r="E65" s="92"/>
-      <c r="F65" s="90"/>
+      <c r="D65" s="75"/>
+      <c r="E65" s="76"/>
+      <c r="F65" s="74"/>
       <c r="G65" s="4"/>
       <c r="H65" s="12"/>
       <c r="I65" s="22"/>
     </row>
     <row r="66" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="27"/>
-      <c r="B66" s="94" t="s">
+      <c r="A66" s="91"/>
+      <c r="B66" s="87" t="s">
         <v>129</v>
       </c>
-      <c r="C66" s="93" t="s">
+      <c r="C66" s="77" t="s">
         <v>127</v>
       </c>
-      <c r="D66" s="91"/>
-      <c r="E66" s="92"/>
-      <c r="F66" s="90"/>
+      <c r="D66" s="75"/>
+      <c r="E66" s="76"/>
+      <c r="F66" s="74"/>
       <c r="G66" s="4"/>
       <c r="H66" s="12"/>
       <c r="I66" s="22"/>
     </row>
     <row r="67" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="27"/>
-      <c r="B67" s="95"/>
-      <c r="C67" s="93" t="s">
+      <c r="A67" s="91"/>
+      <c r="B67" s="88"/>
+      <c r="C67" s="77" t="s">
         <v>126</v>
       </c>
-      <c r="D67" s="91"/>
-      <c r="E67" s="92"/>
-      <c r="F67" s="90"/>
+      <c r="D67" s="75"/>
+      <c r="E67" s="76"/>
+      <c r="F67" s="74"/>
       <c r="G67" s="4"/>
       <c r="H67" s="12"/>
       <c r="I67" s="22"/>
     </row>
     <row r="68" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="27"/>
-      <c r="B68" s="96"/>
-      <c r="C68" s="93" t="s">
+      <c r="A68" s="91"/>
+      <c r="B68" s="89"/>
+      <c r="C68" s="77" t="s">
         <v>128</v>
       </c>
-      <c r="D68" s="91"/>
-      <c r="E68" s="92"/>
-      <c r="F68" s="90"/>
+      <c r="D68" s="75"/>
+      <c r="E68" s="76"/>
+      <c r="F68" s="74"/>
       <c r="G68" s="4"/>
       <c r="H68" s="12"/>
       <c r="I68" s="22"/>
     </row>
     <row r="69" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="27"/>
-      <c r="B69" s="88">
+      <c r="A69" s="91"/>
+      <c r="B69" s="72">
         <v>1</v>
       </c>
-      <c r="C69" s="93" t="s">
+      <c r="C69" s="77" t="s">
         <v>130</v>
       </c>
-      <c r="D69" s="91"/>
-      <c r="E69" s="92"/>
-      <c r="F69" s="90"/>
+      <c r="D69" s="75"/>
+      <c r="E69" s="76"/>
+      <c r="F69" s="74"/>
       <c r="G69" s="4"/>
       <c r="H69" s="12"/>
       <c r="I69" s="22"/>
     </row>
     <row r="70" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="27"/>
-      <c r="B70" s="88">
+      <c r="A70" s="91"/>
+      <c r="B70" s="72">
         <v>1</v>
       </c>
-      <c r="C70" s="89" t="s">
+      <c r="C70" s="73" t="s">
         <v>131</v>
       </c>
-      <c r="D70" s="91"/>
-      <c r="E70" s="92"/>
-      <c r="F70" s="90"/>
+      <c r="D70" s="75"/>
+      <c r="E70" s="76"/>
+      <c r="F70" s="74"/>
       <c r="G70" s="4"/>
       <c r="H70" s="12"/>
       <c r="I70" s="22"/>
     </row>
     <row r="71" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="27"/>
-      <c r="B71" s="88">
+      <c r="A71" s="91"/>
+      <c r="B71" s="72">
         <v>1</v>
       </c>
-      <c r="C71" s="89" t="s">
+      <c r="C71" s="73" t="s">
         <v>132</v>
       </c>
-      <c r="D71" s="91"/>
-      <c r="E71" s="92"/>
-      <c r="F71" s="90"/>
+      <c r="D71" s="75"/>
+      <c r="E71" s="76"/>
+      <c r="F71" s="74"/>
       <c r="G71" s="4"/>
       <c r="H71" s="12"/>
       <c r="I71" s="22"/>
     </row>
     <row r="72" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="27"/>
-      <c r="B72" s="88">
+      <c r="A72" s="91"/>
+      <c r="B72" s="72">
         <v>1</v>
       </c>
-      <c r="C72" s="89" t="s">
+      <c r="C72" s="73" t="s">
         <v>133</v>
       </c>
-      <c r="D72" s="91"/>
-      <c r="E72" s="92"/>
-      <c r="F72" s="90"/>
+      <c r="D72" s="75"/>
+      <c r="E72" s="76"/>
+      <c r="F72" s="74"/>
       <c r="G72" s="4"/>
       <c r="H72" s="12"/>
       <c r="I72" s="22"/>
     </row>
     <row r="73" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="27"/>
-      <c r="B73" s="88">
+      <c r="A73" s="91"/>
+      <c r="B73" s="72">
         <v>1</v>
       </c>
-      <c r="C73" s="89" t="s">
+      <c r="C73" s="73" t="s">
         <v>134</v>
       </c>
-      <c r="D73" s="91"/>
-      <c r="E73" s="92"/>
-      <c r="F73" s="90"/>
+      <c r="D73" s="75"/>
+      <c r="E73" s="76"/>
+      <c r="F73" s="74"/>
       <c r="G73" s="4"/>
       <c r="H73" s="12"/>
       <c r="I73" s="22"/>
     </row>
     <row r="74" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="27"/>
-      <c r="B74" s="88">
+      <c r="A74" s="91"/>
+      <c r="B74" s="72">
         <v>1</v>
       </c>
-      <c r="C74" s="89" t="s">
+      <c r="C74" s="73" t="s">
         <v>135</v>
       </c>
-      <c r="D74" s="91"/>
-      <c r="E74" s="92"/>
-      <c r="F74" s="90"/>
+      <c r="D74" s="75"/>
+      <c r="E74" s="76"/>
+      <c r="F74" s="74"/>
       <c r="G74" s="4"/>
       <c r="H74" s="12"/>
       <c r="I74" s="22"/>
     </row>
     <row r="75" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="27"/>
-      <c r="B75" s="88">
+      <c r="A75" s="91"/>
+      <c r="B75" s="72">
         <v>1</v>
       </c>
-      <c r="C75" s="89" t="s">
+      <c r="C75" s="73" t="s">
         <v>136</v>
       </c>
-      <c r="D75" s="91"/>
-      <c r="E75" s="92"/>
-      <c r="F75" s="90"/>
+      <c r="D75" s="75"/>
+      <c r="E75" s="76"/>
+      <c r="F75" s="74"/>
       <c r="G75" s="4"/>
       <c r="H75" s="12"/>
       <c r="I75" s="22"/>
     </row>
     <row r="76" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="27"/>
-      <c r="B76" s="88">
+      <c r="A76" s="91"/>
+      <c r="B76" s="72">
         <v>1</v>
       </c>
-      <c r="C76" s="89" t="s">
+      <c r="C76" s="73" t="s">
         <v>137</v>
       </c>
-      <c r="D76" s="91"/>
-      <c r="E76" s="92"/>
-      <c r="F76" s="90"/>
+      <c r="D76" s="75"/>
+      <c r="E76" s="76"/>
+      <c r="F76" s="74"/>
       <c r="G76" s="4"/>
       <c r="H76" s="12"/>
       <c r="I76" s="22"/>
     </row>
     <row r="77" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="27"/>
-      <c r="B77" s="88">
+      <c r="A77" s="91"/>
+      <c r="B77" s="72">
         <v>1</v>
       </c>
-      <c r="C77" s="89" t="s">
+      <c r="C77" s="73" t="s">
         <v>138</v>
       </c>
-      <c r="D77" s="91"/>
-      <c r="E77" s="92"/>
-      <c r="F77" s="90"/>
+      <c r="D77" s="75"/>
+      <c r="E77" s="76"/>
+      <c r="F77" s="74"/>
       <c r="G77" s="4"/>
       <c r="H77" s="12"/>
       <c r="I77" s="22"/>
     </row>
     <row r="78" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="27"/>
-      <c r="B78" s="88">
+      <c r="A78" s="91"/>
+      <c r="B78" s="72">
         <v>1</v>
       </c>
-      <c r="C78" s="89" t="s">
+      <c r="C78" s="73" t="s">
         <v>139</v>
       </c>
-      <c r="D78" s="91"/>
-      <c r="E78" s="92"/>
-      <c r="F78" s="90"/>
+      <c r="D78" s="75"/>
+      <c r="E78" s="76"/>
+      <c r="F78" s="74"/>
       <c r="G78" s="4"/>
       <c r="H78" s="12"/>
       <c r="I78" s="22"/>
     </row>
     <row r="79" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="27"/>
-      <c r="B79" s="88">
+      <c r="A79" s="91"/>
+      <c r="B79" s="72">
         <v>1</v>
       </c>
-      <c r="C79" s="89" t="s">
+      <c r="C79" s="73" t="s">
         <v>140</v>
       </c>
-      <c r="D79" s="91"/>
-      <c r="E79" s="92"/>
-      <c r="F79" s="90"/>
+      <c r="D79" s="75"/>
+      <c r="E79" s="76"/>
+      <c r="F79" s="74"/>
       <c r="G79" s="4"/>
       <c r="H79" s="12"/>
       <c r="I79" s="22"/>
     </row>
     <row r="80" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="27"/>
-      <c r="B80" s="88">
+      <c r="A80" s="91"/>
+      <c r="B80" s="72">
         <v>1</v>
       </c>
-      <c r="C80" s="93" t="s">
+      <c r="C80" s="77" t="s">
         <v>141</v>
       </c>
-      <c r="D80" s="91"/>
-      <c r="E80" s="92"/>
-      <c r="F80" s="90"/>
+      <c r="D80" s="75"/>
+      <c r="E80" s="76"/>
+      <c r="F80" s="74"/>
       <c r="G80" s="4"/>
       <c r="H80" s="12"/>
       <c r="I80" s="22"/>
     </row>
     <row r="81" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="27"/>
-      <c r="B81" s="88">
+      <c r="A81" s="91"/>
+      <c r="B81" s="72">
         <v>1</v>
       </c>
-      <c r="C81" s="89" t="s">
+      <c r="C81" s="73" t="s">
         <v>142</v>
       </c>
-      <c r="D81" s="91"/>
-      <c r="E81" s="92"/>
-      <c r="F81" s="90"/>
+      <c r="D81" s="75"/>
+      <c r="E81" s="76"/>
+      <c r="F81" s="74"/>
       <c r="G81" s="4"/>
       <c r="H81" s="12"/>
       <c r="I81" s="22"/>
     </row>
     <row r="82" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="27"/>
-      <c r="B82" s="88">
+      <c r="A82" s="91"/>
+      <c r="B82" s="72">
         <v>1</v>
       </c>
-      <c r="C82" s="89" t="s">
+      <c r="C82" s="73" t="s">
         <v>143</v>
       </c>
-      <c r="D82" s="91"/>
-      <c r="E82" s="92"/>
-      <c r="F82" s="90"/>
+      <c r="D82" s="75"/>
+      <c r="E82" s="76"/>
+      <c r="F82" s="74"/>
       <c r="G82" s="4"/>
       <c r="H82" s="12"/>
       <c r="I82" s="22"/>
     </row>
     <row r="83" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="27"/>
-      <c r="B83" s="88">
+      <c r="A83" s="91"/>
+      <c r="B83" s="72">
         <v>1</v>
       </c>
-      <c r="C83" s="93" t="s">
+      <c r="C83" s="77" t="s">
         <v>144</v>
       </c>
-      <c r="D83" s="91"/>
-      <c r="E83" s="92"/>
-      <c r="F83" s="90"/>
+      <c r="D83" s="75"/>
+      <c r="E83" s="76"/>
+      <c r="F83" s="74"/>
       <c r="G83" s="4"/>
       <c r="H83" s="12"/>
       <c r="I83" s="22"/>
     </row>
     <row r="84" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="27"/>
-      <c r="B84" s="88">
+      <c r="A84" s="91"/>
+      <c r="B84" s="72">
         <v>1</v>
       </c>
-      <c r="C84" s="93" t="s">
+      <c r="C84" s="77" t="s">
         <v>101</v>
       </c>
-      <c r="D84" s="91"/>
-      <c r="E84" s="92"/>
-      <c r="F84" s="90"/>
+      <c r="D84" s="75"/>
+      <c r="E84" s="76"/>
+      <c r="F84" s="74"/>
       <c r="G84" s="4"/>
       <c r="H84" s="12"/>
       <c r="I84" s="22"/>
     </row>
     <row r="85" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="27"/>
-      <c r="B85" s="88">
+      <c r="A85" s="91"/>
+      <c r="B85" s="72">
         <v>1</v>
       </c>
-      <c r="C85" s="93" t="s">
+      <c r="C85" s="77" t="s">
         <v>145</v>
       </c>
-      <c r="D85" s="91"/>
-      <c r="E85" s="92"/>
-      <c r="F85" s="90"/>
+      <c r="D85" s="75"/>
+      <c r="E85" s="76"/>
+      <c r="F85" s="74"/>
       <c r="G85" s="4"/>
       <c r="H85" s="12"/>
       <c r="I85" s="22"/>
     </row>
     <row r="86" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="27"/>
-      <c r="B86" s="88">
+      <c r="A86" s="91"/>
+      <c r="B86" s="72">
         <v>1</v>
       </c>
-      <c r="C86" s="89" t="s">
+      <c r="C86" s="73" t="s">
         <v>146</v>
       </c>
-      <c r="D86" s="91"/>
-      <c r="E86" s="92"/>
-      <c r="F86" s="90"/>
+      <c r="D86" s="75"/>
+      <c r="E86" s="76"/>
+      <c r="F86" s="74"/>
       <c r="G86" s="4"/>
       <c r="H86" s="12"/>
       <c r="I86" s="22"/>
     </row>
     <row r="87" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="27"/>
-      <c r="B87" s="88">
+      <c r="A87" s="91"/>
+      <c r="B87" s="72">
         <v>1</v>
       </c>
-      <c r="C87" s="93" t="s">
+      <c r="C87" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="D87" s="91"/>
-      <c r="E87" s="92"/>
-      <c r="F87" s="90"/>
+      <c r="D87" s="75"/>
+      <c r="E87" s="76"/>
+      <c r="F87" s="74"/>
       <c r="G87" s="4"/>
       <c r="H87" s="12"/>
       <c r="I87" s="22"/>
     </row>
     <row r="88" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="27"/>
-      <c r="B88" s="88">
+      <c r="A88" s="91"/>
+      <c r="B88" s="72">
         <v>1</v>
       </c>
-      <c r="C88" s="93" t="s">
+      <c r="C88" s="77" t="s">
         <v>100</v>
       </c>
-      <c r="D88" s="91"/>
-      <c r="E88" s="92"/>
-      <c r="F88" s="90"/>
+      <c r="D88" s="75"/>
+      <c r="E88" s="76"/>
+      <c r="F88" s="74"/>
       <c r="G88" s="4"/>
       <c r="H88" s="12"/>
       <c r="I88" s="22"/>
     </row>
     <row r="89" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="27"/>
-      <c r="B89" s="88">
+      <c r="A89" s="91"/>
+      <c r="B89" s="72">
         <v>1</v>
       </c>
-      <c r="C89" s="93" t="s">
+      <c r="C89" s="77" t="s">
         <v>147</v>
       </c>
-      <c r="D89" s="91"/>
-      <c r="E89" s="92"/>
-      <c r="F89" s="90"/>
+      <c r="D89" s="75"/>
+      <c r="E89" s="76"/>
+      <c r="F89" s="74"/>
       <c r="G89" s="4"/>
       <c r="H89" s="12"/>
       <c r="I89" s="22"/>
     </row>
     <row r="90" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="27"/>
-      <c r="B90" s="88">
+      <c r="A90" s="91"/>
+      <c r="B90" s="72">
         <v>1</v>
       </c>
-      <c r="C90" s="93" t="s">
+      <c r="C90" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="D90" s="91"/>
-      <c r="E90" s="92"/>
-      <c r="F90" s="90"/>
+      <c r="D90" s="75"/>
+      <c r="E90" s="76"/>
+      <c r="F90" s="74"/>
       <c r="G90" s="4"/>
       <c r="H90" s="12"/>
       <c r="I90" s="22"/>
     </row>
     <row r="91" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="27"/>
-      <c r="B91" s="88">
+      <c r="A91" s="91"/>
+      <c r="B91" s="72">
         <v>1</v>
       </c>
-      <c r="C91" s="93" t="s">
+      <c r="C91" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="D91" s="91"/>
-      <c r="E91" s="92"/>
-      <c r="F91" s="90"/>
+      <c r="D91" s="75"/>
+      <c r="E91" s="76"/>
+      <c r="F91" s="74"/>
       <c r="G91" s="4"/>
       <c r="H91" s="12"/>
       <c r="I91" s="22"/>
     </row>
     <row r="92" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="27"/>
-      <c r="B92" s="88">
+      <c r="A92" s="91"/>
+      <c r="B92" s="72">
         <v>1</v>
       </c>
-      <c r="C92" s="93" t="s">
+      <c r="C92" s="77" t="s">
         <v>72</v>
       </c>
-      <c r="D92" s="91"/>
-      <c r="E92" s="92"/>
-      <c r="F92" s="90"/>
+      <c r="D92" s="75"/>
+      <c r="E92" s="76"/>
+      <c r="F92" s="74"/>
       <c r="G92" s="4"/>
       <c r="H92" s="12"/>
       <c r="I92" s="22"/>
     </row>
     <row r="93" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="27"/>
-      <c r="B93" s="88">
+      <c r="A93" s="91"/>
+      <c r="B93" s="72">
         <v>1</v>
       </c>
-      <c r="C93" s="93" t="s">
+      <c r="C93" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="D93" s="91"/>
-      <c r="E93" s="92"/>
-      <c r="F93" s="90"/>
+      <c r="D93" s="75"/>
+      <c r="E93" s="76"/>
+      <c r="F93" s="74"/>
       <c r="G93" s="4"/>
       <c r="H93" s="12"/>
       <c r="I93" s="22"/>
     </row>
     <row r="94" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="27"/>
-      <c r="B94" s="88">
+      <c r="A94" s="91"/>
+      <c r="B94" s="72">
         <v>1</v>
       </c>
-      <c r="C94" s="93" t="s">
+      <c r="C94" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="D94" s="91"/>
-      <c r="E94" s="92"/>
-      <c r="F94" s="90"/>
+      <c r="D94" s="75"/>
+      <c r="E94" s="76"/>
+      <c r="F94" s="74"/>
       <c r="G94" s="4"/>
       <c r="H94" s="12"/>
       <c r="I94" s="22"/>
     </row>
     <row r="95" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="27"/>
-      <c r="B95" s="88">
+      <c r="A95" s="91"/>
+      <c r="B95" s="72">
         <v>1</v>
       </c>
-      <c r="C95" s="93" t="s">
+      <c r="C95" s="77" t="s">
         <v>64</v>
       </c>
-      <c r="D95" s="91"/>
-      <c r="E95" s="92"/>
-      <c r="F95" s="90"/>
+      <c r="D95" s="75"/>
+      <c r="E95" s="76"/>
+      <c r="F95" s="74"/>
       <c r="G95" s="4"/>
       <c r="H95" s="12"/>
       <c r="I95" s="22"/>
     </row>
     <row r="96" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="27"/>
-      <c r="B96" s="88">
+      <c r="A96" s="91"/>
+      <c r="B96" s="72">
         <v>1</v>
       </c>
-      <c r="C96" s="93" t="s">
+      <c r="C96" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="D96" s="91"/>
-      <c r="E96" s="92"/>
-      <c r="F96" s="90"/>
+      <c r="D96" s="75"/>
+      <c r="E96" s="76"/>
+      <c r="F96" s="74"/>
       <c r="G96" s="4"/>
       <c r="H96" s="12"/>
       <c r="I96" s="22"/>
     </row>
     <row r="97" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="27"/>
-      <c r="B97" s="88">
+      <c r="A97" s="91"/>
+      <c r="B97" s="72">
         <v>1</v>
       </c>
-      <c r="C97" s="93" t="s">
+      <c r="C97" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="D97" s="91"/>
-      <c r="E97" s="92"/>
-      <c r="F97" s="90"/>
+      <c r="D97" s="75"/>
+      <c r="E97" s="76"/>
+      <c r="F97" s="74"/>
       <c r="G97" s="4"/>
       <c r="H97" s="12"/>
       <c r="I97" s="22"/>
     </row>
     <row r="98" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="27"/>
-      <c r="B98" s="88">
+      <c r="A98" s="91"/>
+      <c r="B98" s="72">
         <v>1</v>
       </c>
-      <c r="C98" s="93" t="s">
+      <c r="C98" s="77" t="s">
         <v>67</v>
       </c>
-      <c r="D98" s="91"/>
-      <c r="E98" s="92"/>
-      <c r="F98" s="90"/>
+      <c r="D98" s="75"/>
+      <c r="E98" s="76"/>
+      <c r="F98" s="74"/>
       <c r="G98" s="4"/>
       <c r="H98" s="12"/>
       <c r="I98" s="22"/>
     </row>
     <row r="99" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="27"/>
-      <c r="B99" s="88">
+      <c r="A99" s="91"/>
+      <c r="B99" s="72">
         <v>1</v>
       </c>
-      <c r="C99" s="93" t="s">
+      <c r="C99" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="D99" s="91"/>
-      <c r="E99" s="92"/>
-      <c r="F99" s="90"/>
+      <c r="D99" s="75"/>
+      <c r="E99" s="76"/>
+      <c r="F99" s="74"/>
       <c r="G99" s="4"/>
       <c r="H99" s="12"/>
       <c r="I99" s="22"/>
     </row>
-    <row r="100" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="27"/>
-      <c r="B100" s="88">
+    <row r="100" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="93"/>
+      <c r="B100" s="72">
         <v>1</v>
       </c>
-      <c r="C100" s="93" t="s">
+      <c r="C100" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="D100" s="91"/>
-      <c r="E100" s="92"/>
-      <c r="F100" s="90"/>
+      <c r="D100" s="75"/>
+      <c r="E100" s="76"/>
+      <c r="F100" s="74"/>
       <c r="G100" s="4"/>
       <c r="H100" s="12"/>
       <c r="I100" s="22"/>
     </row>
     <row r="101" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="27"/>
-      <c r="B101" s="88"/>
-      <c r="C101" s="89"/>
-      <c r="D101" s="91"/>
-      <c r="E101" s="92"/>
-      <c r="F101" s="90"/>
+      <c r="A101" s="92"/>
+      <c r="B101" s="72"/>
+      <c r="C101" s="73"/>
+      <c r="D101" s="75"/>
+      <c r="E101" s="76"/>
+      <c r="F101" s="74"/>
       <c r="G101" s="4"/>
       <c r="H101" s="12"/>
       <c r="I101" s="22"/>
     </row>
     <row r="102" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="27"/>
-      <c r="B102" s="88"/>
-      <c r="C102" s="89"/>
-      <c r="D102" s="91"/>
-      <c r="E102" s="92"/>
-      <c r="F102" s="90"/>
+      <c r="A102" s="5"/>
+      <c r="B102" s="72"/>
+      <c r="C102" s="73"/>
+      <c r="D102" s="75"/>
+      <c r="E102" s="76"/>
+      <c r="F102" s="74"/>
       <c r="G102" s="4"/>
       <c r="H102" s="12"/>
       <c r="I102" s="22"/>
     </row>
     <row r="103" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="27"/>
-      <c r="B103" s="88"/>
-      <c r="C103" s="89"/>
-      <c r="D103" s="91"/>
-      <c r="E103" s="92"/>
-      <c r="F103" s="90"/>
+      <c r="A103" s="5"/>
+      <c r="B103" s="72"/>
+      <c r="C103" s="73"/>
+      <c r="D103" s="75"/>
+      <c r="E103" s="76"/>
+      <c r="F103" s="74"/>
       <c r="G103" s="4"/>
       <c r="H103" s="12"/>
       <c r="I103" s="22"/>
     </row>
     <row r="104" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="27"/>
-      <c r="B104" s="88"/>
-      <c r="C104" s="89"/>
-      <c r="D104" s="91"/>
-      <c r="E104" s="92"/>
-      <c r="F104" s="90"/>
+      <c r="A104" s="5"/>
+      <c r="B104" s="72"/>
+      <c r="C104" s="73"/>
+      <c r="D104" s="75"/>
+      <c r="E104" s="76"/>
+      <c r="F104" s="74"/>
       <c r="G104" s="4"/>
       <c r="H104" s="12"/>
       <c r="I104" s="22"/>
     </row>
     <row r="105" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="27"/>
-      <c r="B105" s="88"/>
-      <c r="C105" s="89"/>
-      <c r="D105" s="91"/>
-      <c r="E105" s="92"/>
-      <c r="F105" s="90"/>
+      <c r="A105" s="5"/>
+      <c r="B105" s="72"/>
+      <c r="C105" s="73"/>
+      <c r="D105" s="75"/>
+      <c r="E105" s="76"/>
+      <c r="F105" s="74"/>
       <c r="G105" s="4"/>
       <c r="H105" s="12"/>
       <c r="I105" s="22"/>
     </row>
     <row r="106" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="27"/>
-      <c r="B106" s="88"/>
-      <c r="C106" s="89"/>
-      <c r="D106" s="91"/>
-      <c r="E106" s="92"/>
-      <c r="F106" s="90"/>
+      <c r="A106" s="5"/>
+      <c r="B106" s="72"/>
+      <c r="C106" s="73"/>
+      <c r="D106" s="75"/>
+      <c r="E106" s="76"/>
+      <c r="F106" s="74"/>
       <c r="G106" s="4"/>
       <c r="H106" s="12"/>
       <c r="I106" s="22"/>
     </row>
     <row r="107" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="27"/>
-      <c r="B107" s="88"/>
-      <c r="C107" s="89"/>
-      <c r="D107" s="91"/>
-      <c r="E107" s="92"/>
-      <c r="F107" s="90"/>
+      <c r="A107" s="5"/>
+      <c r="B107" s="72"/>
+      <c r="C107" s="73"/>
+      <c r="D107" s="75"/>
+      <c r="E107" s="76"/>
+      <c r="F107" s="74"/>
       <c r="G107" s="4"/>
       <c r="H107" s="12"/>
       <c r="I107" s="22"/>
@@ -11727,14 +11715,15 @@
       <c r="H856" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="B66:B68"/>
+    <mergeCell ref="A40:A100"/>
     <mergeCell ref="H5:H6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B1:I3"/>
     <mergeCell ref="A12:A30"/>
     <mergeCell ref="A31:A39"/>
     <mergeCell ref="A5:A11"/>
-    <mergeCell ref="B66:B68"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <hyperlinks>

</xml_diff>